<commit_message>
feature(main): update of results
</commit_message>
<xml_diff>
--- a/data/errors_df.xlsx
+++ b/data/errors_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:QX2"/>
+  <dimension ref="A1:QY2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -936,1607 +936,1607 @@
       </c>
       <c r="CW1" s="1" t="inlineStr">
         <is>
-          <t>CINF.O</t>
+          <t>CTAS.O</t>
         </is>
       </c>
       <c r="CX1" s="1" t="inlineStr">
         <is>
-          <t>CTAS.O</t>
+          <t>CSCO.O</t>
         </is>
       </c>
       <c r="CY1" s="1" t="inlineStr">
         <is>
-          <t>CSCO.O</t>
+          <t>C.N</t>
         </is>
       </c>
       <c r="CZ1" s="1" t="inlineStr">
         <is>
-          <t>C.N</t>
+          <t>CFG.N</t>
         </is>
       </c>
       <c r="DA1" s="1" t="inlineStr">
         <is>
-          <t>CFG.N</t>
+          <t>CLX.N</t>
         </is>
       </c>
       <c r="DB1" s="1" t="inlineStr">
         <is>
-          <t>CLX.N</t>
+          <t>CME.O</t>
         </is>
       </c>
       <c r="DC1" s="1" t="inlineStr">
         <is>
-          <t>CME.O</t>
+          <t>CMS.N</t>
         </is>
       </c>
       <c r="DD1" s="1" t="inlineStr">
         <is>
-          <t>CMS.N</t>
+          <t>KO.N</t>
         </is>
       </c>
       <c r="DE1" s="1" t="inlineStr">
         <is>
-          <t>KO.N</t>
+          <t>CTSH.O</t>
         </is>
       </c>
       <c r="DF1" s="1" t="inlineStr">
         <is>
-          <t>CTSH.O</t>
+          <t>CL.N</t>
         </is>
       </c>
       <c r="DG1" s="1" t="inlineStr">
         <is>
-          <t>CL.N</t>
+          <t>CMCSA.O</t>
         </is>
       </c>
       <c r="DH1" s="1" t="inlineStr">
         <is>
-          <t>CMCSA.O</t>
+          <t>CAG.N</t>
         </is>
       </c>
       <c r="DI1" s="1" t="inlineStr">
         <is>
-          <t>CAG.N</t>
+          <t>COP.N</t>
         </is>
       </c>
       <c r="DJ1" s="1" t="inlineStr">
         <is>
-          <t>COP.N</t>
+          <t>ED.N</t>
         </is>
       </c>
       <c r="DK1" s="1" t="inlineStr">
         <is>
-          <t>ED.N</t>
+          <t>STZ.N</t>
         </is>
       </c>
       <c r="DL1" s="1" t="inlineStr">
         <is>
-          <t>STZ.N</t>
+          <t>CPRT.O</t>
         </is>
       </c>
       <c r="DM1" s="1" t="inlineStr">
         <is>
-          <t>CPRT.O</t>
+          <t>GLW.N</t>
         </is>
       </c>
       <c r="DN1" s="1" t="inlineStr">
         <is>
-          <t>GLW.N</t>
+          <t>CPAY.N</t>
         </is>
       </c>
       <c r="DO1" s="1" t="inlineStr">
         <is>
-          <t>CPAY.N</t>
+          <t>CTVA.N</t>
         </is>
       </c>
       <c r="DP1" s="1" t="inlineStr">
         <is>
-          <t>CTVA.N</t>
+          <t>CSGP.O</t>
         </is>
       </c>
       <c r="DQ1" s="1" t="inlineStr">
         <is>
-          <t>CSGP.O</t>
+          <t>COST.O</t>
         </is>
       </c>
       <c r="DR1" s="1" t="inlineStr">
         <is>
-          <t>COST.O</t>
+          <t>CTRA.N</t>
         </is>
       </c>
       <c r="DS1" s="1" t="inlineStr">
         <is>
-          <t>CTRA.N</t>
+          <t>CRWD.O</t>
         </is>
       </c>
       <c r="DT1" s="1" t="inlineStr">
         <is>
-          <t>CRWD.O</t>
+          <t>CCI.N</t>
         </is>
       </c>
       <c r="DU1" s="1" t="inlineStr">
         <is>
-          <t>CCI.N</t>
+          <t>CSX.O</t>
         </is>
       </c>
       <c r="DV1" s="1" t="inlineStr">
         <is>
-          <t>CSX.O</t>
+          <t>CMI.N</t>
         </is>
       </c>
       <c r="DW1" s="1" t="inlineStr">
         <is>
-          <t>CMI.N</t>
+          <t>CVS.N</t>
         </is>
       </c>
       <c r="DX1" s="1" t="inlineStr">
         <is>
-          <t>CVS.N</t>
+          <t>DHR.N</t>
         </is>
       </c>
       <c r="DY1" s="1" t="inlineStr">
         <is>
-          <t>DHR.N</t>
+          <t>DRI.N</t>
         </is>
       </c>
       <c r="DZ1" s="1" t="inlineStr">
         <is>
-          <t>DRI.N</t>
+          <t>DVA.N</t>
         </is>
       </c>
       <c r="EA1" s="1" t="inlineStr">
         <is>
-          <t>DVA.N</t>
+          <t>DE.N</t>
         </is>
       </c>
       <c r="EB1" s="1" t="inlineStr">
         <is>
-          <t>DE.N</t>
+          <t>DELL.N</t>
         </is>
       </c>
       <c r="EC1" s="1" t="inlineStr">
         <is>
-          <t>DELL.N</t>
+          <t>DAL.N</t>
         </is>
       </c>
       <c r="ED1" s="1" t="inlineStr">
         <is>
-          <t>DAL.N</t>
+          <t>DVN.N</t>
         </is>
       </c>
       <c r="EE1" s="1" t="inlineStr">
         <is>
-          <t>DVN.N</t>
+          <t>DXCM.O</t>
         </is>
       </c>
       <c r="EF1" s="1" t="inlineStr">
         <is>
-          <t>DXCM.O</t>
+          <t>FANG.O</t>
         </is>
       </c>
       <c r="EG1" s="1" t="inlineStr">
         <is>
-          <t>FANG.O</t>
+          <t>DLR.N</t>
         </is>
       </c>
       <c r="EH1" s="1" t="inlineStr">
         <is>
-          <t>DLR.N</t>
+          <t>DFS.N</t>
         </is>
       </c>
       <c r="EI1" s="1" t="inlineStr">
         <is>
-          <t>DFS.N</t>
+          <t>DG.N</t>
         </is>
       </c>
       <c r="EJ1" s="1" t="inlineStr">
         <is>
-          <t>DG.N</t>
+          <t>DLTR.O</t>
         </is>
       </c>
       <c r="EK1" s="1" t="inlineStr">
         <is>
-          <t>DLTR.O</t>
+          <t>D.N</t>
         </is>
       </c>
       <c r="EL1" s="1" t="inlineStr">
         <is>
-          <t>D.N</t>
+          <t>DPZ.N</t>
         </is>
       </c>
       <c r="EM1" s="1" t="inlineStr">
         <is>
-          <t>DPZ.N</t>
+          <t>DOV.N</t>
         </is>
       </c>
       <c r="EN1" s="1" t="inlineStr">
         <is>
-          <t>DOV.N</t>
+          <t>DOW.N</t>
         </is>
       </c>
       <c r="EO1" s="1" t="inlineStr">
         <is>
-          <t>DOW.N</t>
+          <t>DHI.N</t>
         </is>
       </c>
       <c r="EP1" s="1" t="inlineStr">
         <is>
-          <t>DHI.N</t>
+          <t>DUK.N</t>
         </is>
       </c>
       <c r="EQ1" s="1" t="inlineStr">
         <is>
-          <t>DUK.N</t>
+          <t>DD.N</t>
         </is>
       </c>
       <c r="ER1" s="1" t="inlineStr">
         <is>
-          <t>DD.N</t>
+          <t>EMN.N</t>
         </is>
       </c>
       <c r="ES1" s="1" t="inlineStr">
         <is>
-          <t>EMN.N</t>
+          <t>ETN.N</t>
         </is>
       </c>
       <c r="ET1" s="1" t="inlineStr">
         <is>
-          <t>ETN.N</t>
+          <t>EBAY.O</t>
         </is>
       </c>
       <c r="EU1" s="1" t="inlineStr">
         <is>
-          <t>EBAY.O</t>
+          <t>ECL.N</t>
         </is>
       </c>
       <c r="EV1" s="1" t="inlineStr">
         <is>
-          <t>ECL.N</t>
+          <t>EIX.N</t>
         </is>
       </c>
       <c r="EW1" s="1" t="inlineStr">
         <is>
-          <t>EIX.N</t>
+          <t>EW.N</t>
         </is>
       </c>
       <c r="EX1" s="1" t="inlineStr">
         <is>
-          <t>EW.N</t>
+          <t>EA.O</t>
         </is>
       </c>
       <c r="EY1" s="1" t="inlineStr">
         <is>
-          <t>EA.O</t>
+          <t>ELV.N</t>
         </is>
       </c>
       <c r="EZ1" s="1" t="inlineStr">
         <is>
-          <t>ELV.N</t>
+          <t>EMR.N</t>
         </is>
       </c>
       <c r="FA1" s="1" t="inlineStr">
         <is>
-          <t>EMR.N</t>
+          <t>ENPH.O</t>
         </is>
       </c>
       <c r="FB1" s="1" t="inlineStr">
         <is>
-          <t>ENPH.O</t>
+          <t>ETR.N</t>
         </is>
       </c>
       <c r="FC1" s="1" t="inlineStr">
         <is>
-          <t>ETR.N</t>
+          <t>EOG.N</t>
         </is>
       </c>
       <c r="FD1" s="1" t="inlineStr">
         <is>
-          <t>EOG.N</t>
+          <t>EPAM.N</t>
         </is>
       </c>
       <c r="FE1" s="1" t="inlineStr">
         <is>
-          <t>EPAM.N</t>
+          <t>EQT.N</t>
         </is>
       </c>
       <c r="FF1" s="1" t="inlineStr">
         <is>
-          <t>EQT.N</t>
+          <t>EFX.N</t>
         </is>
       </c>
       <c r="FG1" s="1" t="inlineStr">
         <is>
-          <t>EFX.N</t>
+          <t>EQIX.O</t>
         </is>
       </c>
       <c r="FH1" s="1" t="inlineStr">
         <is>
-          <t>EQIX.O</t>
+          <t>EQR.N</t>
         </is>
       </c>
       <c r="FI1" s="1" t="inlineStr">
         <is>
-          <t>EQR.N</t>
+          <t>ESS.N</t>
         </is>
       </c>
       <c r="FJ1" s="1" t="inlineStr">
         <is>
-          <t>ESS.N</t>
+          <t>EL.N</t>
         </is>
       </c>
       <c r="FK1" s="1" t="inlineStr">
         <is>
-          <t>EL.N</t>
+          <t>EG.N</t>
         </is>
       </c>
       <c r="FL1" s="1" t="inlineStr">
         <is>
-          <t>EG.N</t>
+          <t>EVRG.O</t>
         </is>
       </c>
       <c r="FM1" s="1" t="inlineStr">
         <is>
-          <t>EVRG.O</t>
+          <t>ES.N</t>
         </is>
       </c>
       <c r="FN1" s="1" t="inlineStr">
         <is>
-          <t>ES.N</t>
+          <t>EXC.O</t>
         </is>
       </c>
       <c r="FO1" s="1" t="inlineStr">
         <is>
-          <t>EXC.O</t>
+          <t>EXPE.O</t>
         </is>
       </c>
       <c r="FP1" s="1" t="inlineStr">
         <is>
-          <t>EXPE.O</t>
+          <t>EXR.N</t>
         </is>
       </c>
       <c r="FQ1" s="1" t="inlineStr">
         <is>
-          <t>EXR.N</t>
+          <t>XOM.N</t>
         </is>
       </c>
       <c r="FR1" s="1" t="inlineStr">
         <is>
-          <t>XOM.N</t>
+          <t>FFIV.O</t>
         </is>
       </c>
       <c r="FS1" s="1" t="inlineStr">
         <is>
-          <t>FFIV.O</t>
+          <t>FDS.N</t>
         </is>
       </c>
       <c r="FT1" s="1" t="inlineStr">
         <is>
-          <t>FDS.N</t>
+          <t>FAST.O</t>
         </is>
       </c>
       <c r="FU1" s="1" t="inlineStr">
         <is>
-          <t>FAST.O</t>
+          <t>FRT.N</t>
         </is>
       </c>
       <c r="FV1" s="1" t="inlineStr">
         <is>
-          <t>FRT.N</t>
+          <t>FDX.N</t>
         </is>
       </c>
       <c r="FW1" s="1" t="inlineStr">
         <is>
-          <t>FDX.N</t>
+          <t>FIS.N</t>
         </is>
       </c>
       <c r="FX1" s="1" t="inlineStr">
         <is>
-          <t>FIS.N</t>
+          <t>FITB.O</t>
         </is>
       </c>
       <c r="FY1" s="1" t="inlineStr">
         <is>
-          <t>FITB.O</t>
+          <t>FSLR.O</t>
         </is>
       </c>
       <c r="FZ1" s="1" t="inlineStr">
         <is>
-          <t>FSLR.O</t>
+          <t>FE.N</t>
         </is>
       </c>
       <c r="GA1" s="1" t="inlineStr">
         <is>
-          <t>FE.N</t>
+          <t>FI.N</t>
         </is>
       </c>
       <c r="GB1" s="1" t="inlineStr">
         <is>
-          <t>FI.N</t>
+          <t>FMC.N</t>
         </is>
       </c>
       <c r="GC1" s="1" t="inlineStr">
         <is>
-          <t>FMC.N</t>
+          <t>F.N</t>
         </is>
       </c>
       <c r="GD1" s="1" t="inlineStr">
         <is>
-          <t>F.N</t>
+          <t>FTNT.O</t>
         </is>
       </c>
       <c r="GE1" s="1" t="inlineStr">
         <is>
-          <t>FTNT.O</t>
+          <t>FTV.N</t>
         </is>
       </c>
       <c r="GF1" s="1" t="inlineStr">
         <is>
-          <t>FTV.N</t>
+          <t>FOXA.O</t>
         </is>
       </c>
       <c r="GG1" s="1" t="inlineStr">
         <is>
-          <t>FOXA.O</t>
+          <t>BEN.N</t>
         </is>
       </c>
       <c r="GH1" s="1" t="inlineStr">
         <is>
-          <t>BEN.N</t>
+          <t>FCX.N</t>
         </is>
       </c>
       <c r="GI1" s="1" t="inlineStr">
         <is>
-          <t>FCX.N</t>
+          <t>GRMN.N</t>
         </is>
       </c>
       <c r="GJ1" s="1" t="inlineStr">
         <is>
-          <t>GRMN.N</t>
+          <t>IT.N</t>
         </is>
       </c>
       <c r="GK1" s="1" t="inlineStr">
         <is>
-          <t>IT.N</t>
+          <t>GE.N</t>
         </is>
       </c>
       <c r="GL1" s="1" t="inlineStr">
         <is>
-          <t>GE.N</t>
+          <t>GEN.O</t>
         </is>
       </c>
       <c r="GM1" s="1" t="inlineStr">
         <is>
-          <t>GEN.O</t>
+          <t>GNRC.N</t>
         </is>
       </c>
       <c r="GN1" s="1" t="inlineStr">
         <is>
-          <t>GNRC.N</t>
+          <t>GD.N</t>
         </is>
       </c>
       <c r="GO1" s="1" t="inlineStr">
         <is>
-          <t>GD.N</t>
+          <t>GIS.N</t>
         </is>
       </c>
       <c r="GP1" s="1" t="inlineStr">
         <is>
-          <t>GIS.N</t>
+          <t>GM.N</t>
         </is>
       </c>
       <c r="GQ1" s="1" t="inlineStr">
         <is>
-          <t>GM.N</t>
+          <t>GPC.N</t>
         </is>
       </c>
       <c r="GR1" s="1" t="inlineStr">
         <is>
-          <t>GPC.N</t>
+          <t>GILD.O</t>
         </is>
       </c>
       <c r="GS1" s="1" t="inlineStr">
         <is>
-          <t>GILD.O</t>
+          <t>GPN.N</t>
         </is>
       </c>
       <c r="GT1" s="1" t="inlineStr">
         <is>
-          <t>GPN.N</t>
+          <t>GL.N</t>
         </is>
       </c>
       <c r="GU1" s="1" t="inlineStr">
         <is>
-          <t>GL.N</t>
+          <t>GDDY.N</t>
         </is>
       </c>
       <c r="GV1" s="1" t="inlineStr">
         <is>
-          <t>GDDY.N</t>
+          <t>GS.N</t>
         </is>
       </c>
       <c r="GW1" s="1" t="inlineStr">
         <is>
-          <t>GS.N</t>
+          <t>HAL.N</t>
         </is>
       </c>
       <c r="GX1" s="1" t="inlineStr">
         <is>
-          <t>HAL.N</t>
+          <t>HIG.N</t>
         </is>
       </c>
       <c r="GY1" s="1" t="inlineStr">
         <is>
-          <t>HIG.N</t>
+          <t>HAS.O</t>
         </is>
       </c>
       <c r="GZ1" s="1" t="inlineStr">
         <is>
-          <t>HAS.O</t>
+          <t>HCA.N</t>
         </is>
       </c>
       <c r="HA1" s="1" t="inlineStr">
         <is>
-          <t>HCA.N</t>
+          <t>DOC.N</t>
         </is>
       </c>
       <c r="HB1" s="1" t="inlineStr">
         <is>
-          <t>DOC.N</t>
+          <t>HSIC.O</t>
         </is>
       </c>
       <c r="HC1" s="1" t="inlineStr">
         <is>
-          <t>HSIC.O</t>
+          <t>HSY.N</t>
         </is>
       </c>
       <c r="HD1" s="1" t="inlineStr">
         <is>
-          <t>HSY.N</t>
+          <t>HES.N</t>
         </is>
       </c>
       <c r="HE1" s="1" t="inlineStr">
         <is>
-          <t>HES.N</t>
+          <t>HPE.N</t>
         </is>
       </c>
       <c r="HF1" s="1" t="inlineStr">
         <is>
-          <t>HPE.N</t>
+          <t>HLT.N</t>
         </is>
       </c>
       <c r="HG1" s="1" t="inlineStr">
         <is>
-          <t>HLT.N</t>
+          <t>HOLX.O</t>
         </is>
       </c>
       <c r="HH1" s="1" t="inlineStr">
         <is>
-          <t>HOLX.O</t>
+          <t>HON.O</t>
         </is>
       </c>
       <c r="HI1" s="1" t="inlineStr">
         <is>
-          <t>HD.N</t>
+          <t>HRL.N</t>
         </is>
       </c>
       <c r="HJ1" s="1" t="inlineStr">
         <is>
-          <t>HON.O</t>
+          <t>HST.O</t>
         </is>
       </c>
       <c r="HK1" s="1" t="inlineStr">
         <is>
-          <t>HRL.N</t>
+          <t>HWM.N</t>
         </is>
       </c>
       <c r="HL1" s="1" t="inlineStr">
         <is>
-          <t>HST.O</t>
+          <t>HPQ.N</t>
         </is>
       </c>
       <c r="HM1" s="1" t="inlineStr">
         <is>
-          <t>HWM.N</t>
+          <t>HUM.N</t>
         </is>
       </c>
       <c r="HN1" s="1" t="inlineStr">
         <is>
-          <t>HPQ.N</t>
+          <t>HBAN.O</t>
         </is>
       </c>
       <c r="HO1" s="1" t="inlineStr">
         <is>
-          <t>HUM.N</t>
+          <t>HII.N</t>
         </is>
       </c>
       <c r="HP1" s="1" t="inlineStr">
         <is>
-          <t>HBAN.O</t>
+          <t>IBM.N</t>
         </is>
       </c>
       <c r="HQ1" s="1" t="inlineStr">
         <is>
-          <t>HII.N</t>
+          <t>IEX.N</t>
         </is>
       </c>
       <c r="HR1" s="1" t="inlineStr">
         <is>
-          <t>IBM.N</t>
+          <t>IDXX.O</t>
         </is>
       </c>
       <c r="HS1" s="1" t="inlineStr">
         <is>
-          <t>IEX.N</t>
+          <t>ITW.N</t>
         </is>
       </c>
       <c r="HT1" s="1" t="inlineStr">
         <is>
-          <t>IDXX.O</t>
+          <t>INCY.O</t>
         </is>
       </c>
       <c r="HU1" s="1" t="inlineStr">
         <is>
-          <t>ITW.N</t>
+          <t>IR.N</t>
         </is>
       </c>
       <c r="HV1" s="1" t="inlineStr">
         <is>
-          <t>INCY.O</t>
+          <t>PODD.O</t>
         </is>
       </c>
       <c r="HW1" s="1" t="inlineStr">
         <is>
-          <t>IR.N</t>
+          <t>INTC.O</t>
         </is>
       </c>
       <c r="HX1" s="1" t="inlineStr">
         <is>
-          <t>PODD.O</t>
+          <t>ICE.N</t>
         </is>
       </c>
       <c r="HY1" s="1" t="inlineStr">
         <is>
-          <t>INTC.O</t>
+          <t>IFF.N</t>
         </is>
       </c>
       <c r="HZ1" s="1" t="inlineStr">
         <is>
-          <t>ICE.N</t>
+          <t>IP.N</t>
         </is>
       </c>
       <c r="IA1" s="1" t="inlineStr">
         <is>
-          <t>IFF.N</t>
+          <t>IPG.N</t>
         </is>
       </c>
       <c r="IB1" s="1" t="inlineStr">
         <is>
-          <t>IP.N</t>
+          <t>INTU.O</t>
         </is>
       </c>
       <c r="IC1" s="1" t="inlineStr">
         <is>
-          <t>IPG.N</t>
+          <t>ISRG.O</t>
         </is>
       </c>
       <c r="ID1" s="1" t="inlineStr">
         <is>
-          <t>INTU.O</t>
+          <t>IVZ.N</t>
         </is>
       </c>
       <c r="IE1" s="1" t="inlineStr">
         <is>
-          <t>ISRG.O</t>
+          <t>INVH.N</t>
         </is>
       </c>
       <c r="IF1" s="1" t="inlineStr">
         <is>
-          <t>IVZ.N</t>
+          <t>IQV.N</t>
         </is>
       </c>
       <c r="IG1" s="1" t="inlineStr">
         <is>
-          <t>INVH.N</t>
+          <t>IRM.N</t>
         </is>
       </c>
       <c r="IH1" s="1" t="inlineStr">
         <is>
-          <t>IQV.N</t>
+          <t>JBHT.O</t>
         </is>
       </c>
       <c r="II1" s="1" t="inlineStr">
         <is>
-          <t>IRM.N</t>
+          <t>JKHY.O</t>
         </is>
       </c>
       <c r="IJ1" s="1" t="inlineStr">
         <is>
-          <t>JBHT.O</t>
+          <t>J.N</t>
         </is>
       </c>
       <c r="IK1" s="1" t="inlineStr">
         <is>
-          <t>JKHY.O</t>
+          <t>JNJ.N</t>
         </is>
       </c>
       <c r="IL1" s="1" t="inlineStr">
         <is>
-          <t>J.N</t>
+          <t>JCI.N</t>
         </is>
       </c>
       <c r="IM1" s="1" t="inlineStr">
         <is>
-          <t>JNJ.N</t>
+          <t>JPM.N</t>
         </is>
       </c>
       <c r="IN1" s="1" t="inlineStr">
         <is>
-          <t>JCI.N</t>
+          <t>JNPR.N</t>
         </is>
       </c>
       <c r="IO1" s="1" t="inlineStr">
         <is>
-          <t>JPM.N</t>
+          <t>KDP.O</t>
         </is>
       </c>
       <c r="IP1" s="1" t="inlineStr">
         <is>
-          <t>JNPR.N</t>
+          <t>KEY.N</t>
         </is>
       </c>
       <c r="IQ1" s="1" t="inlineStr">
         <is>
-          <t>KDP.O</t>
+          <t>KEYS.N</t>
         </is>
       </c>
       <c r="IR1" s="1" t="inlineStr">
         <is>
-          <t>KEY.N</t>
+          <t>KMB.N</t>
         </is>
       </c>
       <c r="IS1" s="1" t="inlineStr">
         <is>
-          <t>KEYS.N</t>
+          <t>KIM.N</t>
         </is>
       </c>
       <c r="IT1" s="1" t="inlineStr">
         <is>
-          <t>KMB.N</t>
+          <t>KMI.N</t>
         </is>
       </c>
       <c r="IU1" s="1" t="inlineStr">
         <is>
-          <t>KIM.N</t>
+          <t>KLAC.O</t>
         </is>
       </c>
       <c r="IV1" s="1" t="inlineStr">
         <is>
-          <t>KMI.N</t>
+          <t>KHC.O</t>
         </is>
       </c>
       <c r="IW1" s="1" t="inlineStr">
         <is>
-          <t>KLAC.O</t>
+          <t>KR.N</t>
         </is>
       </c>
       <c r="IX1" s="1" t="inlineStr">
         <is>
-          <t>KHC.O</t>
+          <t>LHX.N</t>
         </is>
       </c>
       <c r="IY1" s="1" t="inlineStr">
         <is>
-          <t>KR.N</t>
+          <t>LH.N</t>
         </is>
       </c>
       <c r="IZ1" s="1" t="inlineStr">
         <is>
-          <t>LHX.N</t>
+          <t>LRCX.O</t>
         </is>
       </c>
       <c r="JA1" s="1" t="inlineStr">
         <is>
-          <t>LH.N</t>
+          <t>LW.N</t>
         </is>
       </c>
       <c r="JB1" s="1" t="inlineStr">
         <is>
-          <t>LRCX.O</t>
+          <t>LVS.N</t>
         </is>
       </c>
       <c r="JC1" s="1" t="inlineStr">
         <is>
-          <t>LW.N</t>
+          <t>LDOS.N</t>
         </is>
       </c>
       <c r="JD1" s="1" t="inlineStr">
         <is>
-          <t>LVS.N</t>
+          <t>LLY.N</t>
         </is>
       </c>
       <c r="JE1" s="1" t="inlineStr">
         <is>
-          <t>LDOS.N</t>
+          <t>LYV.N</t>
         </is>
       </c>
       <c r="JF1" s="1" t="inlineStr">
         <is>
-          <t>LLY.N</t>
+          <t>LKQ.O</t>
         </is>
       </c>
       <c r="JG1" s="1" t="inlineStr">
         <is>
-          <t>LYV.N</t>
+          <t>LMT.N</t>
         </is>
       </c>
       <c r="JH1" s="1" t="inlineStr">
         <is>
-          <t>LKQ.O</t>
+          <t>LOW.N</t>
         </is>
       </c>
       <c r="JI1" s="1" t="inlineStr">
         <is>
-          <t>LMT.N</t>
+          <t>LULU.O</t>
         </is>
       </c>
       <c r="JJ1" s="1" t="inlineStr">
         <is>
-          <t>LOW.N</t>
+          <t>LYB.N</t>
         </is>
       </c>
       <c r="JK1" s="1" t="inlineStr">
         <is>
-          <t>LULU.O</t>
+          <t>MTB.N</t>
         </is>
       </c>
       <c r="JL1" s="1" t="inlineStr">
         <is>
-          <t>LYB.N</t>
+          <t>MRO.N</t>
         </is>
       </c>
       <c r="JM1" s="1" t="inlineStr">
         <is>
-          <t>MTB.N</t>
+          <t>MPC.N</t>
         </is>
       </c>
       <c r="JN1" s="1" t="inlineStr">
         <is>
-          <t>MRO.N</t>
+          <t>MKTX.O</t>
         </is>
       </c>
       <c r="JO1" s="1" t="inlineStr">
         <is>
-          <t>MPC.N</t>
+          <t>MAR.O</t>
         </is>
       </c>
       <c r="JP1" s="1" t="inlineStr">
         <is>
-          <t>MKTX.O</t>
+          <t>MMC.N</t>
         </is>
       </c>
       <c r="JQ1" s="1" t="inlineStr">
         <is>
-          <t>MAR.O</t>
+          <t>MLM.N</t>
         </is>
       </c>
       <c r="JR1" s="1" t="inlineStr">
         <is>
-          <t>MMC.N</t>
+          <t>MAS.N</t>
         </is>
       </c>
       <c r="JS1" s="1" t="inlineStr">
         <is>
-          <t>MLM.N</t>
+          <t>MA.N</t>
         </is>
       </c>
       <c r="JT1" s="1" t="inlineStr">
         <is>
-          <t>MAS.N</t>
+          <t>MTCH.O</t>
         </is>
       </c>
       <c r="JU1" s="1" t="inlineStr">
         <is>
-          <t>MA.N</t>
+          <t>MKC.N</t>
         </is>
       </c>
       <c r="JV1" s="1" t="inlineStr">
         <is>
-          <t>MTCH.O</t>
+          <t>MCD.N</t>
         </is>
       </c>
       <c r="JW1" s="1" t="inlineStr">
         <is>
-          <t>MKC.N</t>
+          <t>MCK.N</t>
         </is>
       </c>
       <c r="JX1" s="1" t="inlineStr">
         <is>
-          <t>MCD.N</t>
+          <t>MDT.N</t>
         </is>
       </c>
       <c r="JY1" s="1" t="inlineStr">
         <is>
-          <t>MCK.N</t>
+          <t>MRK.N</t>
         </is>
       </c>
       <c r="JZ1" s="1" t="inlineStr">
         <is>
-          <t>MDT.N</t>
+          <t>META.O</t>
         </is>
       </c>
       <c r="KA1" s="1" t="inlineStr">
         <is>
-          <t>MRK.N</t>
+          <t>MET.N</t>
         </is>
       </c>
       <c r="KB1" s="1" t="inlineStr">
         <is>
-          <t>META.O</t>
+          <t>MTD.N</t>
         </is>
       </c>
       <c r="KC1" s="1" t="inlineStr">
         <is>
-          <t>MET.N</t>
+          <t>MGM.N</t>
         </is>
       </c>
       <c r="KD1" s="1" t="inlineStr">
         <is>
-          <t>MTD.N</t>
+          <t>MCHP.O</t>
         </is>
       </c>
       <c r="KE1" s="1" t="inlineStr">
         <is>
-          <t>MGM.N</t>
+          <t>MU.O</t>
         </is>
       </c>
       <c r="KF1" s="1" t="inlineStr">
         <is>
-          <t>MCHP.O</t>
+          <t>MSFT.O</t>
         </is>
       </c>
       <c r="KG1" s="1" t="inlineStr">
         <is>
-          <t>MU.O</t>
+          <t>MAA.N</t>
         </is>
       </c>
       <c r="KH1" s="1" t="inlineStr">
         <is>
-          <t>MSFT.O</t>
+          <t>MRNA.O</t>
         </is>
       </c>
       <c r="KI1" s="1" t="inlineStr">
         <is>
-          <t>MAA.N</t>
+          <t>MHK.N</t>
         </is>
       </c>
       <c r="KJ1" s="1" t="inlineStr">
         <is>
-          <t>MRNA.O</t>
+          <t>MOH.N</t>
         </is>
       </c>
       <c r="KK1" s="1" t="inlineStr">
         <is>
-          <t>MHK.N</t>
+          <t>TAP.N</t>
         </is>
       </c>
       <c r="KL1" s="1" t="inlineStr">
         <is>
-          <t>MOH.N</t>
+          <t>MDLZ.O</t>
         </is>
       </c>
       <c r="KM1" s="1" t="inlineStr">
         <is>
-          <t>TAP.N</t>
+          <t>MPWR.O</t>
         </is>
       </c>
       <c r="KN1" s="1" t="inlineStr">
         <is>
-          <t>MDLZ.O</t>
+          <t>MNST.O</t>
         </is>
       </c>
       <c r="KO1" s="1" t="inlineStr">
         <is>
-          <t>MPWR.O</t>
+          <t>MCO.N</t>
         </is>
       </c>
       <c r="KP1" s="1" t="inlineStr">
         <is>
-          <t>MNST.O</t>
+          <t>MS.N</t>
         </is>
       </c>
       <c r="KQ1" s="1" t="inlineStr">
         <is>
-          <t>MCO.N</t>
+          <t>MOS.N</t>
         </is>
       </c>
       <c r="KR1" s="1" t="inlineStr">
         <is>
-          <t>MS.N</t>
+          <t>MSI.N</t>
         </is>
       </c>
       <c r="KS1" s="1" t="inlineStr">
         <is>
-          <t>MOS.N</t>
+          <t>MSCI.N</t>
         </is>
       </c>
       <c r="KT1" s="1" t="inlineStr">
         <is>
-          <t>MSI.N</t>
+          <t>NDAQ.O</t>
         </is>
       </c>
       <c r="KU1" s="1" t="inlineStr">
         <is>
-          <t>MSCI.N</t>
+          <t>NTAP.O</t>
         </is>
       </c>
       <c r="KV1" s="1" t="inlineStr">
         <is>
-          <t>NDAQ.O</t>
+          <t>NFLX.O</t>
         </is>
       </c>
       <c r="KW1" s="1" t="inlineStr">
         <is>
-          <t>NTAP.O</t>
+          <t>NEM.N</t>
         </is>
       </c>
       <c r="KX1" s="1" t="inlineStr">
         <is>
-          <t>NFLX.O</t>
+          <t>NWSA.O</t>
         </is>
       </c>
       <c r="KY1" s="1" t="inlineStr">
         <is>
-          <t>NEM.N</t>
+          <t>NEE.N</t>
         </is>
       </c>
       <c r="KZ1" s="1" t="inlineStr">
         <is>
-          <t>NWSA.O</t>
+          <t>NKE.N</t>
         </is>
       </c>
       <c r="LA1" s="1" t="inlineStr">
         <is>
-          <t>NEE.N</t>
+          <t>NI.N</t>
         </is>
       </c>
       <c r="LB1" s="1" t="inlineStr">
         <is>
-          <t>NKE.N</t>
+          <t>NDSN.O</t>
         </is>
       </c>
       <c r="LC1" s="1" t="inlineStr">
         <is>
-          <t>NI.N</t>
+          <t>NSC.N</t>
         </is>
       </c>
       <c r="LD1" s="1" t="inlineStr">
         <is>
-          <t>NDSN.O</t>
+          <t>NTRS.O</t>
         </is>
       </c>
       <c r="LE1" s="1" t="inlineStr">
         <is>
-          <t>NSC.N</t>
+          <t>NOC.N</t>
         </is>
       </c>
       <c r="LF1" s="1" t="inlineStr">
         <is>
-          <t>NTRS.O</t>
+          <t>NCLH.N</t>
         </is>
       </c>
       <c r="LG1" s="1" t="inlineStr">
         <is>
-          <t>NCLH.N</t>
+          <t>NRG.N</t>
         </is>
       </c>
       <c r="LH1" s="1" t="inlineStr">
         <is>
-          <t>NRG.N</t>
+          <t>NUE.N</t>
         </is>
       </c>
       <c r="LI1" s="1" t="inlineStr">
         <is>
-          <t>NUE.N</t>
+          <t>NVDA.O</t>
         </is>
       </c>
       <c r="LJ1" s="1" t="inlineStr">
         <is>
-          <t>NVDA.O</t>
+          <t>NVR.N</t>
         </is>
       </c>
       <c r="LK1" s="1" t="inlineStr">
         <is>
-          <t>NVR.N</t>
+          <t>NXPI.O</t>
         </is>
       </c>
       <c r="LL1" s="1" t="inlineStr">
         <is>
-          <t>NXPI.O</t>
+          <t>ORLY.O</t>
         </is>
       </c>
       <c r="LM1" s="1" t="inlineStr">
         <is>
-          <t>ORLY.O</t>
+          <t>OXY.N</t>
         </is>
       </c>
       <c r="LN1" s="1" t="inlineStr">
         <is>
-          <t>OXY.N</t>
+          <t>ODFL.O</t>
         </is>
       </c>
       <c r="LO1" s="1" t="inlineStr">
         <is>
-          <t>ODFL.O</t>
+          <t>OMC.N</t>
         </is>
       </c>
       <c r="LP1" s="1" t="inlineStr">
         <is>
-          <t>OMC.N</t>
+          <t>ON.O</t>
         </is>
       </c>
       <c r="LQ1" s="1" t="inlineStr">
         <is>
-          <t>ON.O</t>
+          <t>OKE.N</t>
         </is>
       </c>
       <c r="LR1" s="1" t="inlineStr">
         <is>
-          <t>OKE.N</t>
+          <t>ORCL.N</t>
         </is>
       </c>
       <c r="LS1" s="1" t="inlineStr">
         <is>
-          <t>ORCL.N</t>
+          <t>OTIS.N</t>
         </is>
       </c>
       <c r="LT1" s="1" t="inlineStr">
         <is>
-          <t>OTIS.N</t>
+          <t>PCAR.O</t>
         </is>
       </c>
       <c r="LU1" s="1" t="inlineStr">
         <is>
-          <t>PCAR.O</t>
+          <t>PKG.N</t>
         </is>
       </c>
       <c r="LV1" s="1" t="inlineStr">
         <is>
-          <t>PKG.N</t>
+          <t>PLTR.N</t>
         </is>
       </c>
       <c r="LW1" s="1" t="inlineStr">
         <is>
-          <t>PLTR.N</t>
+          <t>PANW.N</t>
         </is>
       </c>
       <c r="LX1" s="1" t="inlineStr">
         <is>
-          <t>PANW.N</t>
+          <t>PARA.O</t>
         </is>
       </c>
       <c r="LY1" s="1" t="inlineStr">
         <is>
-          <t>PARA.O</t>
+          <t>PH.N</t>
         </is>
       </c>
       <c r="LZ1" s="1" t="inlineStr">
         <is>
-          <t>PH.N</t>
+          <t>PAYX.O</t>
         </is>
       </c>
       <c r="MA1" s="1" t="inlineStr">
         <is>
-          <t>PAYX.O</t>
+          <t>PAYC.N</t>
         </is>
       </c>
       <c r="MB1" s="1" t="inlineStr">
         <is>
-          <t>PAYC.N</t>
+          <t>PYPL.O</t>
         </is>
       </c>
       <c r="MC1" s="1" t="inlineStr">
         <is>
-          <t>PYPL.O</t>
+          <t>PNR.N</t>
         </is>
       </c>
       <c r="MD1" s="1" t="inlineStr">
         <is>
-          <t>PNR.N</t>
+          <t>PEP.O</t>
         </is>
       </c>
       <c r="ME1" s="1" t="inlineStr">
         <is>
-          <t>PEP.O</t>
+          <t>PFE.N</t>
         </is>
       </c>
       <c r="MF1" s="1" t="inlineStr">
         <is>
-          <t>PFE.N</t>
+          <t>PCG.N</t>
         </is>
       </c>
       <c r="MG1" s="1" t="inlineStr">
         <is>
-          <t>PCG.N</t>
+          <t>PM.N</t>
         </is>
       </c>
       <c r="MH1" s="1" t="inlineStr">
         <is>
-          <t>PM.N</t>
+          <t>PSX.N</t>
         </is>
       </c>
       <c r="MI1" s="1" t="inlineStr">
         <is>
-          <t>PSX.N</t>
+          <t>PNW.N</t>
         </is>
       </c>
       <c r="MJ1" s="1" t="inlineStr">
         <is>
-          <t>PNW.N</t>
+          <t>PNC.N</t>
         </is>
       </c>
       <c r="MK1" s="1" t="inlineStr">
         <is>
-          <t>PNC.N</t>
+          <t>POOL.O</t>
         </is>
       </c>
       <c r="ML1" s="1" t="inlineStr">
         <is>
-          <t>POOL.O</t>
+          <t>PPG.N</t>
         </is>
       </c>
       <c r="MM1" s="1" t="inlineStr">
         <is>
-          <t>PPG.N</t>
+          <t>PPL.N</t>
         </is>
       </c>
       <c r="MN1" s="1" t="inlineStr">
         <is>
-          <t>PPL.N</t>
+          <t>PFG.O</t>
         </is>
       </c>
       <c r="MO1" s="1" t="inlineStr">
         <is>
-          <t>PFG.O</t>
+          <t>PG.N</t>
         </is>
       </c>
       <c r="MP1" s="1" t="inlineStr">
         <is>
-          <t>PG.N</t>
+          <t>PGR.N</t>
         </is>
       </c>
       <c r="MQ1" s="1" t="inlineStr">
         <is>
-          <t>PGR.N</t>
+          <t>PLD.N</t>
         </is>
       </c>
       <c r="MR1" s="1" t="inlineStr">
         <is>
-          <t>PLD.N</t>
+          <t>PRU.N</t>
         </is>
       </c>
       <c r="MS1" s="1" t="inlineStr">
         <is>
-          <t>PRU.N</t>
+          <t>PEG.N</t>
         </is>
       </c>
       <c r="MT1" s="1" t="inlineStr">
         <is>
-          <t>PEG.N</t>
+          <t>PTC.O</t>
         </is>
       </c>
       <c r="MU1" s="1" t="inlineStr">
         <is>
-          <t>PTC.O</t>
+          <t>PSA.N</t>
         </is>
       </c>
       <c r="MV1" s="1" t="inlineStr">
         <is>
-          <t>PSA.N</t>
+          <t>PHM.N</t>
         </is>
       </c>
       <c r="MW1" s="1" t="inlineStr">
         <is>
-          <t>PHM.N</t>
+          <t>QRVO.O</t>
         </is>
       </c>
       <c r="MX1" s="1" t="inlineStr">
         <is>
-          <t>QRVO.O</t>
+          <t>PWR.N</t>
         </is>
       </c>
       <c r="MY1" s="1" t="inlineStr">
         <is>
-          <t>PWR.N</t>
+          <t>QCOM.O</t>
         </is>
       </c>
       <c r="MZ1" s="1" t="inlineStr">
         <is>
-          <t>QCOM.O</t>
+          <t>DGX.N</t>
         </is>
       </c>
       <c r="NA1" s="1" t="inlineStr">
         <is>
-          <t>DGX.N</t>
+          <t>RL.N</t>
         </is>
       </c>
       <c r="NB1" s="1" t="inlineStr">
         <is>
-          <t>RL.N</t>
+          <t>RJF.N</t>
         </is>
       </c>
       <c r="NC1" s="1" t="inlineStr">
         <is>
-          <t>RJF.N</t>
+          <t>RTX.N</t>
         </is>
       </c>
       <c r="ND1" s="1" t="inlineStr">
         <is>
-          <t>RTX.N</t>
+          <t>REG.O</t>
         </is>
       </c>
       <c r="NE1" s="1" t="inlineStr">
         <is>
-          <t>REG.O</t>
+          <t>REGN.O</t>
         </is>
       </c>
       <c r="NF1" s="1" t="inlineStr">
         <is>
-          <t>REGN.O</t>
+          <t>RF.N</t>
         </is>
       </c>
       <c r="NG1" s="1" t="inlineStr">
         <is>
-          <t>RF.N</t>
+          <t>RSG.N</t>
         </is>
       </c>
       <c r="NH1" s="1" t="inlineStr">
         <is>
-          <t>RSG.N</t>
+          <t>RMD.N</t>
         </is>
       </c>
       <c r="NI1" s="1" t="inlineStr">
         <is>
-          <t>RMD.N</t>
+          <t>RVTY.N</t>
         </is>
       </c>
       <c r="NJ1" s="1" t="inlineStr">
         <is>
-          <t>RVTY.N</t>
+          <t>ROK.N</t>
         </is>
       </c>
       <c r="NK1" s="1" t="inlineStr">
         <is>
-          <t>ROK.N</t>
+          <t>ROL.N</t>
         </is>
       </c>
       <c r="NL1" s="1" t="inlineStr">
         <is>
-          <t>ROL.N</t>
+          <t>ROP.O</t>
         </is>
       </c>
       <c r="NM1" s="1" t="inlineStr">
         <is>
-          <t>ROP.O</t>
+          <t>ROST.O</t>
         </is>
       </c>
       <c r="NN1" s="1" t="inlineStr">
         <is>
-          <t>ROST.O</t>
+          <t>RCL.N</t>
         </is>
       </c>
       <c r="NO1" s="1" t="inlineStr">
         <is>
-          <t>RCL.N</t>
+          <t>SPGI.N</t>
         </is>
       </c>
       <c r="NP1" s="1" t="inlineStr">
         <is>
-          <t>SPGI.N</t>
+          <t>CRM.N</t>
         </is>
       </c>
       <c r="NQ1" s="1" t="inlineStr">
         <is>
-          <t>CRM.N</t>
+          <t>SBAC.O</t>
         </is>
       </c>
       <c r="NR1" s="1" t="inlineStr">
         <is>
-          <t>SBAC.O</t>
+          <t>SLB.N</t>
         </is>
       </c>
       <c r="NS1" s="1" t="inlineStr">
         <is>
-          <t>SLB.N</t>
+          <t>STX.O</t>
         </is>
       </c>
       <c r="NT1" s="1" t="inlineStr">
         <is>
-          <t>STX.O</t>
+          <t>SRE.N</t>
         </is>
       </c>
       <c r="NU1" s="1" t="inlineStr">
         <is>
-          <t>SRE.N</t>
+          <t>NOW.N</t>
         </is>
       </c>
       <c r="NV1" s="1" t="inlineStr">
         <is>
-          <t>NOW.N</t>
+          <t>SHW.N</t>
         </is>
       </c>
       <c r="NW1" s="1" t="inlineStr">
         <is>
-          <t>SHW.N</t>
+          <t>SPG.N</t>
         </is>
       </c>
       <c r="NX1" s="1" t="inlineStr">
         <is>
-          <t>SPG.N</t>
+          <t>SWKS.O</t>
         </is>
       </c>
       <c r="NY1" s="1" t="inlineStr">
         <is>
-          <t>SWKS.O</t>
+          <t>SJM.N</t>
         </is>
       </c>
       <c r="NZ1" s="1" t="inlineStr">
         <is>
-          <t>SJM.N</t>
+          <t>SNA.N</t>
         </is>
       </c>
       <c r="OA1" s="1" t="inlineStr">
         <is>
-          <t>SNA.N</t>
+          <t>SO.N</t>
         </is>
       </c>
       <c r="OB1" s="1" t="inlineStr">
         <is>
-          <t>SO.N</t>
+          <t>LUV.N</t>
         </is>
       </c>
       <c r="OC1" s="1" t="inlineStr">
         <is>
-          <t>LUV.N</t>
+          <t>STT.N</t>
         </is>
       </c>
       <c r="OD1" s="1" t="inlineStr">
         <is>
-          <t>SBUX.O</t>
+          <t>STLD.O</t>
         </is>
       </c>
       <c r="OE1" s="1" t="inlineStr">
         <is>
-          <t>STT.N</t>
+          <t>STE.N</t>
         </is>
       </c>
       <c r="OF1" s="1" t="inlineStr">
         <is>
-          <t>STLD.O</t>
+          <t>SYK.N</t>
         </is>
       </c>
       <c r="OG1" s="1" t="inlineStr">
         <is>
-          <t>STE.N</t>
+          <t>SMCI.O</t>
         </is>
       </c>
       <c r="OH1" s="1" t="inlineStr">
         <is>
-          <t>SYK.N</t>
+          <t>SYF.N</t>
         </is>
       </c>
       <c r="OI1" s="1" t="inlineStr">
         <is>
-          <t>SMCI.O</t>
+          <t>SNPS.O</t>
         </is>
       </c>
       <c r="OJ1" s="1" t="inlineStr">
         <is>
-          <t>SYF.N</t>
+          <t>SYY.N</t>
         </is>
       </c>
       <c r="OK1" s="1" t="inlineStr">
         <is>
-          <t>SNPS.O</t>
+          <t>TMUS.O</t>
         </is>
       </c>
       <c r="OL1" s="1" t="inlineStr">
         <is>
-          <t>SYY.N</t>
+          <t>TROW.O</t>
         </is>
       </c>
       <c r="OM1" s="1" t="inlineStr">
         <is>
-          <t>TMUS.O</t>
+          <t>TTWO.O</t>
         </is>
       </c>
       <c r="ON1" s="1" t="inlineStr">
         <is>
-          <t>TROW.O</t>
+          <t>TPR.N</t>
         </is>
       </c>
       <c r="OO1" s="1" t="inlineStr">
         <is>
-          <t>TTWO.O</t>
+          <t>TRGP.N</t>
         </is>
       </c>
       <c r="OP1" s="1" t="inlineStr">
         <is>
-          <t>TPR.N</t>
+          <t>TGT.N</t>
         </is>
       </c>
       <c r="OQ1" s="1" t="inlineStr">
         <is>
-          <t>TRGP.N</t>
+          <t>TEL.N</t>
         </is>
       </c>
       <c r="OR1" s="1" t="inlineStr">
         <is>
-          <t>TGT.N</t>
+          <t>TDY.N</t>
         </is>
       </c>
       <c r="OS1" s="1" t="inlineStr">
         <is>
-          <t>TEL.N</t>
+          <t>TFX.N</t>
         </is>
       </c>
       <c r="OT1" s="1" t="inlineStr">
         <is>
-          <t>TDY.N</t>
+          <t>TER.O</t>
         </is>
       </c>
       <c r="OU1" s="1" t="inlineStr">
         <is>
-          <t>TFX.N</t>
+          <t>TSLA.O</t>
         </is>
       </c>
       <c r="OV1" s="1" t="inlineStr">
         <is>
-          <t>TER.O</t>
+          <t>TXN.O</t>
         </is>
       </c>
       <c r="OW1" s="1" t="inlineStr">
         <is>
-          <t>TSLA.O</t>
+          <t>TXT.N</t>
         </is>
       </c>
       <c r="OX1" s="1" t="inlineStr">
         <is>
-          <t>TXN.O</t>
+          <t>TMO.N</t>
         </is>
       </c>
       <c r="OY1" s="1" t="inlineStr">
         <is>
-          <t>TXT.N</t>
+          <t>TJX.N</t>
         </is>
       </c>
       <c r="OZ1" s="1" t="inlineStr">
         <is>
-          <t>TMO.N</t>
+          <t>TSCO.O</t>
         </is>
       </c>
       <c r="PA1" s="1" t="inlineStr">
         <is>
-          <t>TJX.N</t>
+          <t>TT.N</t>
         </is>
       </c>
       <c r="PB1" s="1" t="inlineStr">
         <is>
-          <t>TSCO.O</t>
+          <t>TDG.N</t>
         </is>
       </c>
       <c r="PC1" s="1" t="inlineStr">
         <is>
-          <t>TDG.N</t>
+          <t>TRV.N</t>
         </is>
       </c>
       <c r="PD1" s="1" t="inlineStr">
         <is>
-          <t>TRV.N</t>
+          <t>TRMB.O</t>
         </is>
       </c>
       <c r="PE1" s="1" t="inlineStr">
         <is>
-          <t>TRMB.O</t>
+          <t>TFC.N</t>
         </is>
       </c>
       <c r="PF1" s="1" t="inlineStr">
@@ -2691,75 +2691,80 @@
       </c>
       <c r="QJ1" s="1" t="inlineStr">
         <is>
+          <t>WAT.N</t>
+        </is>
+      </c>
+      <c r="QK1" s="1" t="inlineStr">
+        <is>
           <t>WEC.N</t>
         </is>
       </c>
-      <c r="QK1" s="1" t="inlineStr">
+      <c r="QL1" s="1" t="inlineStr">
         <is>
           <t>WFC.N</t>
         </is>
       </c>
-      <c r="QL1" s="1" t="inlineStr">
+      <c r="QM1" s="1" t="inlineStr">
         <is>
           <t>WELL.N</t>
         </is>
       </c>
-      <c r="QM1" s="1" t="inlineStr">
+      <c r="QN1" s="1" t="inlineStr">
         <is>
           <t>WST.N</t>
         </is>
       </c>
-      <c r="QN1" s="1" t="inlineStr">
+      <c r="QO1" s="1" t="inlineStr">
         <is>
           <t>WDC.O</t>
         </is>
       </c>
-      <c r="QO1" s="1" t="inlineStr">
+      <c r="QP1" s="1" t="inlineStr">
         <is>
           <t>WY.N</t>
         </is>
       </c>
-      <c r="QP1" s="1" t="inlineStr">
+      <c r="QQ1" s="1" t="inlineStr">
         <is>
           <t>WMB.N</t>
         </is>
       </c>
-      <c r="QQ1" s="1" t="inlineStr">
+      <c r="QR1" s="1" t="inlineStr">
         <is>
           <t>WTW.O</t>
         </is>
       </c>
-      <c r="QR1" s="1" t="inlineStr">
+      <c r="QS1" s="1" t="inlineStr">
         <is>
           <t>WYNN.O</t>
         </is>
       </c>
-      <c r="QS1" s="1" t="inlineStr">
+      <c r="QT1" s="1" t="inlineStr">
         <is>
           <t>XEL.O</t>
         </is>
       </c>
-      <c r="QT1" s="1" t="inlineStr">
+      <c r="QU1" s="1" t="inlineStr">
         <is>
           <t>XYL.N</t>
         </is>
       </c>
-      <c r="QU1" s="1" t="inlineStr">
+      <c r="QV1" s="1" t="inlineStr">
         <is>
           <t>YUM.N</t>
         </is>
       </c>
-      <c r="QV1" s="1" t="inlineStr">
+      <c r="QW1" s="1" t="inlineStr">
         <is>
           <t>ZBRA.O</t>
         </is>
       </c>
-      <c r="QW1" s="1" t="inlineStr">
+      <c r="QX1" s="1" t="inlineStr">
         <is>
           <t>ZBH.N</t>
         </is>
       </c>
-      <c r="QX1" s="1" t="inlineStr">
+      <c r="QY1" s="1" t="inlineStr">
         <is>
           <t>ZTS.N</t>
         </is>
@@ -2767,1402 +2772,1405 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.0622007523906993</v>
+        <v>0.06450018880329585</v>
       </c>
       <c r="B2" t="n">
-        <v>0.05773057142786521</v>
+        <v>0.06675407105421034</v>
       </c>
       <c r="C2" t="n">
-        <v>0.03965400849008962</v>
+        <v>0.04782893812953815</v>
       </c>
       <c r="D2" t="n">
-        <v>0.03884278315802694</v>
+        <v>0.02589163842887846</v>
       </c>
       <c r="E2" t="n">
-        <v>0.02467698617011179</v>
+        <v>0.03057850057734292</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1222933561306818</v>
+        <v>0.1804376175047629</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1498122830901411</v>
+        <v>0.152700486728462</v>
       </c>
       <c r="H2" t="n">
-        <v>0.08886809082670862</v>
+        <v>0.1344285798963518</v>
       </c>
       <c r="I2" t="n">
-        <v>0.03087151650000438</v>
+        <v>0.03426906337702922</v>
       </c>
       <c r="J2" t="n">
-        <v>0.03936458276111179</v>
+        <v>0.04341665247845868</v>
       </c>
       <c r="K2" t="n">
-        <v>0.04886169811213757</v>
+        <v>0.05118603597533591</v>
       </c>
       <c r="L2" t="n">
-        <v>0.02488383238760697</v>
+        <v>0.02087944108525693</v>
       </c>
       <c r="M2" t="n">
-        <v>0.03138048742986608</v>
+        <v>0.03512312428072815</v>
       </c>
       <c r="N2" t="n">
-        <v>0.0830321157636766</v>
+        <v>0.1574855955460459</v>
       </c>
       <c r="O2" t="n">
-        <v>0.06115426443399939</v>
+        <v>0.0609953801260227</v>
       </c>
       <c r="P2" t="n">
-        <v>0.04332308377642576</v>
+        <v>0.06205636225340407</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.05230707426680542</v>
+        <v>0.06982551703158413</v>
       </c>
       <c r="R2" t="n">
-        <v>0.02007009489986678</v>
+        <v>0.0168730275223204</v>
       </c>
       <c r="S2" t="n">
-        <v>0.0291687487681134</v>
+        <v>0.04377860661876178</v>
       </c>
       <c r="T2" t="n">
-        <v>0.09012546400768631</v>
+        <v>0.02875991855296898</v>
       </c>
       <c r="U2" t="n">
-        <v>0.02947065185515995</v>
+        <v>0.02977414614414193</v>
       </c>
       <c r="V2" t="n">
-        <v>0.1164632285065852</v>
+        <v>0.02561673148517939</v>
       </c>
       <c r="W2" t="n">
-        <v>0.05333308215267522</v>
+        <v>0.05000068550249213</v>
       </c>
       <c r="X2" t="n">
-        <v>0.02600636264921068</v>
+        <v>0.03059212639274953</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.03638446899396058</v>
+        <v>0.03807483837597154</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.02553514233781307</v>
+        <v>0.02780314989366046</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.02395785596178338</v>
+        <v>0.01628052734086124</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.1097687822914382</v>
+        <v>0.08978801467829631</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.07481350235768985</v>
+        <v>0.06539006450970238</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.03590035473727093</v>
+        <v>0.02839752471221791</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.04045648087550924</v>
+        <v>0.03309820799439664</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.05666786925274103</v>
+        <v>0.04580422732035382</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.02762261114857903</v>
+        <v>0.03607599811620369</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.01932514309341038</v>
+        <v>0.02438301484105554</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.01482498921476982</v>
+        <v>0.01901422603209207</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.03769481028839563</v>
+        <v>0.02818940527565018</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.03839929185581877</v>
+        <v>0.04644193470248634</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.05444750526671924</v>
+        <v>0.04341786795162951</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.0501890168730505</v>
+        <v>0.04247892328684318</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.08175779236554483</v>
+        <v>0.02489114186992347</v>
       </c>
       <c r="AO2" t="n">
-        <v>0.06826618793213277</v>
+        <v>0.03840118360987236</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.02429990733912245</v>
+        <v>0.02329246993005716</v>
       </c>
       <c r="AQ2" t="n">
-        <v>0.1057304592875395</v>
+        <v>0.09436832956151327</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.03336553492506143</v>
+        <v>0.03395840564699899</v>
       </c>
       <c r="AS2" t="n">
-        <v>0.02840545521808364</v>
+        <v>0.03659697731313151</v>
       </c>
       <c r="AT2" t="n">
-        <v>0.03784280065628417</v>
+        <v>0.01506878988915738</v>
       </c>
       <c r="AU2" t="n">
-        <v>0.0336562141645364</v>
+        <v>0.01879083863405791</v>
       </c>
       <c r="AV2" t="n">
-        <v>0.01932077834424262</v>
+        <v>0.01846409441510145</v>
       </c>
       <c r="AW2" t="n">
-        <v>0.05188280001718889</v>
+        <v>0.02175540756498489</v>
       </c>
       <c r="AX2" t="n">
-        <v>0.02353462535829691</v>
+        <v>0.03357249825596524</v>
       </c>
       <c r="AY2" t="n">
-        <v>0.05685752487034415</v>
+        <v>0.07686145357585175</v>
       </c>
       <c r="AZ2" t="n">
-        <v>0.04445393140093369</v>
+        <v>0.06753998998065443</v>
       </c>
       <c r="BA2" t="n">
-        <v>0.04405504535069702</v>
+        <v>0.05187392034488836</v>
       </c>
       <c r="BB2" t="n">
-        <v>0.1039151817046216</v>
+        <v>0.05677474843835262</v>
       </c>
       <c r="BC2" t="n">
-        <v>0.01996239357316244</v>
+        <v>0.02842959681738931</v>
       </c>
       <c r="BD2" t="n">
-        <v>0.08589060741446745</v>
+        <v>0.04751091464175533</v>
       </c>
       <c r="BE2" t="n">
-        <v>0.03081453317001773</v>
+        <v>0.02880141296163123</v>
       </c>
       <c r="BF2" t="n">
-        <v>0.03079278797200718</v>
+        <v>0.03098870232904958</v>
       </c>
       <c r="BG2" t="n">
-        <v>0.02244652096868459</v>
+        <v>0.02510341602499725</v>
       </c>
       <c r="BH2" t="n">
-        <v>0.05918103340210479</v>
+        <v>0.04225959951741944</v>
       </c>
       <c r="BI2" t="n">
-        <v>0.02244200330524101</v>
+        <v>0.02927601618833072</v>
       </c>
       <c r="BJ2" t="n">
-        <v>0.04972605386339402</v>
+        <v>0.07159154028555663</v>
       </c>
       <c r="BK2" t="n">
-        <v>0.03994620617039719</v>
+        <v>0.04488429844189494</v>
       </c>
       <c r="BL2" t="n">
-        <v>0.07949960612397249</v>
+        <v>0.04381175408909106</v>
       </c>
       <c r="BM2" t="n">
-        <v>0.03065024054675185</v>
+        <v>0.070889027074981</v>
       </c>
       <c r="BN2" t="n">
-        <v>0.04731526340407477</v>
+        <v>0.07065150051883022</v>
       </c>
       <c r="BO2" t="n">
-        <v>0.04425704136641136</v>
+        <v>0.05845231066464886</v>
       </c>
       <c r="BP2" t="n">
-        <v>0.01863148489923621</v>
+        <v>0.02064655017686969</v>
       </c>
       <c r="BQ2" t="n">
-        <v>0.2071006587449818</v>
+        <v>0.2381000318096097</v>
       </c>
       <c r="BR2" t="n">
-        <v>0.02516912503549126</v>
+        <v>0.02418555372084139</v>
       </c>
       <c r="BS2" t="n">
-        <v>0.1001202995932504</v>
+        <v>0.1050978267206009</v>
       </c>
       <c r="BT2" t="n">
-        <v>0.08103444896309867</v>
+        <v>0.09524531446869741</v>
       </c>
       <c r="BU2" t="n">
-        <v>0.02908442576209718</v>
+        <v>0.04000901739109168</v>
       </c>
       <c r="BV2" t="n">
-        <v>0.02521228190058368</v>
+        <v>0.02255122987564566</v>
       </c>
       <c r="BW2" t="n">
-        <v>0.09791632633173912</v>
+        <v>0.09395741256372947</v>
       </c>
       <c r="BX2" t="n">
-        <v>0.03257484366740179</v>
+        <v>0.0489970708453164</v>
       </c>
       <c r="BY2" t="n">
-        <v>0.07407575373579386</v>
+        <v>0.08607974196136065</v>
       </c>
       <c r="BZ2" t="n">
-        <v>0.04348106702466123</v>
+        <v>0.05063589352718323</v>
       </c>
       <c r="CA2" t="n">
-        <v>0.03119799328568399</v>
+        <v>0.03105913076391325</v>
       </c>
       <c r="CB2" t="n">
-        <v>0.0408166961276051</v>
+        <v>0.05680405688193848</v>
       </c>
       <c r="CC2" t="n">
-        <v>0.03925879465268992</v>
+        <v>0.0430819333902832</v>
       </c>
       <c r="CD2" t="n">
-        <v>0.06850620258157473</v>
+        <v>0.0971167642653957</v>
       </c>
       <c r="CE2" t="n">
-        <v>0.02041433871224449</v>
+        <v>0.02608156644535402</v>
       </c>
       <c r="CF2" t="n">
-        <v>0.04423835716207898</v>
+        <v>0.05658427759869089</v>
       </c>
       <c r="CG2" t="n">
-        <v>0.02978191050638868</v>
+        <v>0.03900521267128014</v>
       </c>
       <c r="CH2" t="n">
-        <v>0.03912603548598211</v>
+        <v>0.04513602321264375</v>
       </c>
       <c r="CI2" t="n">
-        <v>0.03862569913693823</v>
+        <v>0.04789024570104106</v>
       </c>
       <c r="CJ2" t="n">
-        <v>0.07378638672420561</v>
+        <v>0.03124850342523849</v>
       </c>
       <c r="CK2" t="n">
-        <v>0.03703314536163655</v>
+        <v>0.03655078217729821</v>
       </c>
       <c r="CL2" t="n">
-        <v>0.04002123244584994</v>
+        <v>0.04699750874189768</v>
       </c>
       <c r="CM2" t="n">
-        <v>0.07097492795790589</v>
+        <v>0.01557562354044257</v>
       </c>
       <c r="CN2" t="n">
-        <v>0.04390151388813072</v>
+        <v>0.0325948737710112</v>
       </c>
       <c r="CO2" t="n">
-        <v>0.08829800468777474</v>
+        <v>0.1164175420379798</v>
       </c>
       <c r="CP2" t="n">
-        <v>0.04837504634410014</v>
+        <v>0.0589134552016275</v>
       </c>
       <c r="CQ2" t="n">
-        <v>0.04720764616138355</v>
+        <v>0.05150198296259492</v>
       </c>
       <c r="CR2" t="n">
-        <v>0.03436644243611754</v>
+        <v>0.03249058205856672</v>
       </c>
       <c r="CS2" t="n">
-        <v>0.03869719852147696</v>
+        <v>0.06884616717742416</v>
       </c>
       <c r="CT2" t="n">
-        <v>0.03182306692678864</v>
+        <v>0.03275260939506484</v>
       </c>
       <c r="CU2" t="n">
-        <v>0.01998523231623648</v>
+        <v>0.01381929040339849</v>
       </c>
       <c r="CV2" t="n">
-        <v>0.1060387283488772</v>
+        <v>0.09497117051141457</v>
       </c>
       <c r="CW2" t="n">
-        <v>0.06784736862486318</v>
+        <v>0.08157283798861503</v>
       </c>
       <c r="CX2" t="n">
-        <v>0.1029009861399574</v>
+        <v>0.01774721618737322</v>
       </c>
       <c r="CY2" t="n">
-        <v>0.02804920256860377</v>
+        <v>0.06194351349473733</v>
       </c>
       <c r="CZ2" t="n">
-        <v>0.1187067034524447</v>
+        <v>0.04020148409205487</v>
       </c>
       <c r="DA2" t="n">
-        <v>0.03281616431057337</v>
+        <v>0.02781566118412124</v>
       </c>
       <c r="DB2" t="n">
-        <v>0.02337759967159236</v>
+        <v>0.01894324238239815</v>
       </c>
       <c r="DC2" t="n">
-        <v>0.0263064014241404</v>
+        <v>0.02445486177778732</v>
       </c>
       <c r="DD2" t="n">
-        <v>0.01858670891015218</v>
+        <v>0.01688975159054154</v>
       </c>
       <c r="DE2" t="n">
-        <v>0.04617508868176671</v>
+        <v>0.03301227933900221</v>
       </c>
       <c r="DF2" t="n">
-        <v>0.0238085597105035</v>
+        <v>0.05418298392543498</v>
       </c>
       <c r="DG2" t="n">
-        <v>0.05853249408189373</v>
+        <v>0.07929640748896853</v>
       </c>
       <c r="DH2" t="n">
-        <v>0.1269683961577068</v>
+        <v>0.0485735719997057</v>
       </c>
       <c r="DI2" t="n">
-        <v>0.03157327040701077</v>
+        <v>0.06079863545480642</v>
       </c>
       <c r="DJ2" t="n">
-        <v>0.05714496728565122</v>
+        <v>0.05368745694536324</v>
       </c>
       <c r="DK2" t="n">
-        <v>0.05680907326734198</v>
+        <v>0.2281354825119984</v>
       </c>
       <c r="DL2" t="n">
-        <v>0.1601358733795614</v>
+        <v>0.07030202564975097</v>
       </c>
       <c r="DM2" t="n">
-        <v>0.03663238292214849</v>
+        <v>0.04016701846125319</v>
       </c>
       <c r="DN2" t="n">
-        <v>0.03648068470686312</v>
+        <v>0.04837669844235967</v>
       </c>
       <c r="DO2" t="n">
-        <v>0.04220492352264561</v>
+        <v>0.04941090614427806</v>
       </c>
       <c r="DP2" t="n">
-        <v>0.0405864334629961</v>
+        <v>0.04265277739795474</v>
       </c>
       <c r="DQ2" t="n">
-        <v>0.03955210936499062</v>
+        <v>0.04083495028751928</v>
       </c>
       <c r="DR2" t="n">
-        <v>0.03199482774519598</v>
+        <v>0.05159989449781227</v>
       </c>
       <c r="DS2" t="n">
-        <v>0.03841951602006934</v>
+        <v>0.05123708738691209</v>
       </c>
       <c r="DT2" t="n">
-        <v>0.05892941387156037</v>
+        <v>0.1089091795194033</v>
       </c>
       <c r="DU2" t="n">
-        <v>0.1535816436948062</v>
+        <v>0.05675565933104618</v>
       </c>
       <c r="DV2" t="n">
-        <v>0.0464553769341623</v>
+        <v>0.03515618879910769</v>
       </c>
       <c r="DW2" t="n">
-        <v>0.02410411027755767</v>
+        <v>0.1020811903596575</v>
       </c>
       <c r="DX2" t="n">
-        <v>0.1216816154953375</v>
+        <v>0.04332451700433824</v>
       </c>
       <c r="DY2" t="n">
-        <v>0.03550652533882967</v>
+        <v>0.09153489904377346</v>
       </c>
       <c r="DZ2" t="n">
-        <v>0.07681356598978425</v>
+        <v>0.05971964831745673</v>
       </c>
       <c r="EA2" t="n">
-        <v>0.06212177129980688</v>
+        <v>0.04214665627747817</v>
       </c>
       <c r="EB2" t="n">
-        <v>0.04968387622223319</v>
+        <v>0.07186010815516239</v>
       </c>
       <c r="EC2" t="n">
-        <v>0.06815308541003158</v>
+        <v>0.04934703333969121</v>
       </c>
       <c r="ED2" t="n">
-        <v>0.0425259938380554</v>
+        <v>0.05641140844504933</v>
       </c>
       <c r="EE2" t="n">
-        <v>0.08673806370252711</v>
+        <v>0.04910163574291806</v>
       </c>
       <c r="EF2" t="n">
-        <v>0.05169709544968946</v>
+        <v>0.04241525879884403</v>
       </c>
       <c r="EG2" t="n">
-        <v>0.07829253592268128</v>
+        <v>0.07813368194552371</v>
       </c>
       <c r="EH2" t="n">
-        <v>0.04241837460559584</v>
+        <v>0.05880701671856279</v>
       </c>
       <c r="EI2" t="n">
-        <v>0.04742226804085634</v>
+        <v>0.04057120827565375</v>
       </c>
       <c r="EJ2" t="n">
-        <v>0.04089362276704501</v>
+        <v>0.0300350188113646</v>
       </c>
       <c r="EK2" t="n">
-        <v>0.07385199689999469</v>
+        <v>0.04242710077661923</v>
       </c>
       <c r="EL2" t="n">
-        <v>0.04228543428012802</v>
+        <v>0.04988365332730388</v>
       </c>
       <c r="EM2" t="n">
-        <v>0.04305802936948457</v>
+        <v>0.04534617433596895</v>
       </c>
       <c r="EN2" t="n">
-        <v>0.0352008859221711</v>
+        <v>0.04785428005791458</v>
       </c>
       <c r="EO2" t="n">
-        <v>0.1164484807480055</v>
+        <v>0.0961320849458332</v>
       </c>
       <c r="EP2" t="n">
-        <v>0.1186725456935807</v>
+        <v>0.03495915304029779</v>
       </c>
       <c r="EQ2" t="n">
-        <v>0.02833356697031355</v>
+        <v>0.08053342818281792</v>
       </c>
       <c r="ER2" t="n">
-        <v>0.06042814776705652</v>
+        <v>0.07180085907966738</v>
       </c>
       <c r="ES2" t="n">
-        <v>0.05962588803208553</v>
+        <v>0.08348907546700472</v>
       </c>
       <c r="ET2" t="n">
-        <v>0.07056861262321505</v>
+        <v>0.03895037013567741</v>
       </c>
       <c r="EU2" t="n">
-        <v>0.04173558026629951</v>
+        <v>0.03223019392448103</v>
       </c>
       <c r="EV2" t="n">
-        <v>0.02098150231530822</v>
+        <v>0.3181639664446418</v>
       </c>
       <c r="EW2" t="n">
-        <v>0.1996323482501384</v>
+        <v>0.01939020880543577</v>
       </c>
       <c r="EX2" t="n">
-        <v>0.02478725069371798</v>
+        <v>0.1306723959126594</v>
       </c>
       <c r="EY2" t="n">
-        <v>0.09209342455884727</v>
+        <v>0.03446337104602205</v>
       </c>
       <c r="EZ2" t="n">
-        <v>0.04051460590910261</v>
+        <v>0.04670406643204946</v>
       </c>
       <c r="FA2" t="n">
-        <v>0.03146938646426872</v>
+        <v>0.06836197816653303</v>
       </c>
       <c r="FB2" t="n">
-        <v>0.03467603979922067</v>
+        <v>0.04456698096012605</v>
       </c>
       <c r="FC2" t="n">
-        <v>0.04324979078391372</v>
+        <v>0.03630936286259654</v>
       </c>
       <c r="FD2" t="n">
-        <v>0.0310674211306016</v>
+        <v>0.04055120985000432</v>
       </c>
       <c r="FE2" t="n">
-        <v>0.03744817555131415</v>
+        <v>0.05886372608002612</v>
       </c>
       <c r="FF2" t="n">
-        <v>0.05685165830441402</v>
+        <v>0.03435107101278066</v>
       </c>
       <c r="FG2" t="n">
-        <v>0.07156932609530396</v>
+        <v>0.03725738129199484</v>
       </c>
       <c r="FH2" t="n">
-        <v>0.02155717370280681</v>
+        <v>0.04001973178407462</v>
       </c>
       <c r="FI2" t="n">
-        <v>0.03233325767889879</v>
+        <v>0.04589620441436624</v>
       </c>
       <c r="FJ2" t="n">
-        <v>0.02320457300720535</v>
+        <v>0.05782625058407546</v>
       </c>
       <c r="FK2" t="n">
-        <v>0.05719211145861233</v>
+        <v>0.05036586987745586</v>
       </c>
       <c r="FL2" t="n">
-        <v>0.03715046058672718</v>
+        <v>0.02145549805282392</v>
       </c>
       <c r="FM2" t="n">
-        <v>0.02005032750008102</v>
+        <v>0.08858192382734628</v>
       </c>
       <c r="FN2" t="n">
-        <v>0.07866144556602246</v>
+        <v>0.03587892145625707</v>
       </c>
       <c r="FO2" t="n">
-        <v>0.03434118768724017</v>
+        <v>0.05133982475071068</v>
       </c>
       <c r="FP2" t="n">
-        <v>0.03539893515250998</v>
+        <v>0.0597926082546494</v>
       </c>
       <c r="FQ2" t="n">
-        <v>0.07300877582157499</v>
+        <v>0.0431580463433909</v>
       </c>
       <c r="FR2" t="n">
-        <v>0.07652825019792506</v>
+        <v>0.04724190854370776</v>
       </c>
       <c r="FS2" t="n">
-        <v>0.04796509446412216</v>
+        <v>0.02673598329400808</v>
       </c>
       <c r="FT2" t="n">
-        <v>0.02688949694961731</v>
+        <v>0.07240357447648153</v>
       </c>
       <c r="FU2" t="n">
-        <v>0.09756562018551719</v>
+        <v>0.04450661841258478</v>
       </c>
       <c r="FV2" t="n">
-        <v>0.0254212738398005</v>
+        <v>0.03674670267073214</v>
       </c>
       <c r="FW2" t="n">
-        <v>0.04293213130294319</v>
+        <v>0.06163422083150273</v>
       </c>
       <c r="FX2" t="n">
-        <v>0.05217601041210279</v>
+        <v>0.07003403584282933</v>
       </c>
       <c r="FY2" t="n">
-        <v>0.06541290047312273</v>
+        <v>0.1233925668325498</v>
       </c>
       <c r="FZ2" t="n">
-        <v>0.05484733654420348</v>
+        <v>0.02938990101126599</v>
       </c>
       <c r="GA2" t="n">
-        <v>0.02973711998845882</v>
+        <v>0.02554780936544409</v>
       </c>
       <c r="GB2" t="n">
-        <v>0.04302878912295528</v>
+        <v>0.1847091832704159</v>
       </c>
       <c r="GC2" t="n">
-        <v>0.1547249742153746</v>
+        <v>0.07048151807643886</v>
       </c>
       <c r="GD2" t="n">
-        <v>0.08911248306878639</v>
+        <v>0.03161080199647166</v>
       </c>
       <c r="GE2" t="n">
-        <v>0.04679011069028299</v>
+        <v>0.02026645436119202</v>
       </c>
       <c r="GF2" t="n">
-        <v>0.04070082390457141</v>
+        <v>0.04448866068802597</v>
       </c>
       <c r="GG2" t="n">
-        <v>0.04158305610672777</v>
+        <v>0.02891618322848917</v>
       </c>
       <c r="GH2" t="n">
-        <v>0.05225393271203193</v>
+        <v>0.1509445032482774</v>
       </c>
       <c r="GI2" t="n">
-        <v>0.111888448981553</v>
+        <v>0.02164098973601258</v>
       </c>
       <c r="GJ2" t="n">
-        <v>0.02020263629575216</v>
+        <v>0.03226499043566891</v>
       </c>
       <c r="GK2" t="n">
-        <v>0.031413202291334</v>
+        <v>0.07175337862266015</v>
       </c>
       <c r="GL2" t="n">
-        <v>0.06216370564342116</v>
+        <v>0.1127300000425493</v>
       </c>
       <c r="GM2" t="n">
-        <v>0.05803491072958264</v>
+        <v>0.1287163626954087</v>
       </c>
       <c r="GN2" t="n">
-        <v>0.1463383641061257</v>
+        <v>0.01728085031954942</v>
       </c>
       <c r="GO2" t="n">
-        <v>0.07270293304300239</v>
+        <v>0.07864776007467297</v>
       </c>
       <c r="GP2" t="n">
-        <v>0.06769973977397062</v>
+        <v>0.03849986913872135</v>
       </c>
       <c r="GQ2" t="n">
-        <v>0.06630238477918919</v>
+        <v>0.05828386275792712</v>
       </c>
       <c r="GR2" t="n">
-        <v>0.03768033400645528</v>
+        <v>0.0220817926029837</v>
       </c>
       <c r="GS2" t="n">
-        <v>0.03067425296311816</v>
+        <v>0.04695450583652377</v>
       </c>
       <c r="GT2" t="n">
-        <v>0.02140497015435893</v>
+        <v>0.06178110465811395</v>
       </c>
       <c r="GU2" t="n">
-        <v>0.04665422129944118</v>
+        <v>0.02604031242424958</v>
       </c>
       <c r="GV2" t="n">
-        <v>0.0564476891651558</v>
+        <v>0.05214105492126819</v>
       </c>
       <c r="GW2" t="n">
-        <v>0.0409991055802346</v>
+        <v>0.0955529088830355</v>
       </c>
       <c r="GX2" t="n">
-        <v>0.06810577921809795</v>
+        <v>0.04805154549009764</v>
       </c>
       <c r="GY2" t="n">
-        <v>0.03557191940262755</v>
+        <v>0.1223669089694466</v>
       </c>
       <c r="GZ2" t="n">
-        <v>0.06847844860167172</v>
+        <v>0.0355335848695484</v>
       </c>
       <c r="HA2" t="n">
-        <v>0.07137328476430566</v>
+        <v>0.06779987096667892</v>
       </c>
       <c r="HB2" t="n">
-        <v>0.04193702798232831</v>
+        <v>0.04829833875629454</v>
       </c>
       <c r="HC2" t="n">
-        <v>0.04882198715894151</v>
+        <v>0.1171763420210271</v>
       </c>
       <c r="HD2" t="n">
-        <v>0.07728373670019768</v>
+        <v>0.04300816385002439</v>
       </c>
       <c r="HE2" t="n">
-        <v>0.03261728447870377</v>
+        <v>0.03490532779957602</v>
       </c>
       <c r="HF2" t="n">
-        <v>0.07616567634778161</v>
+        <v>0.02577449045507327</v>
       </c>
       <c r="HG2" t="n">
-        <v>0.01968608675284887</v>
+        <v>0.07849543208370009</v>
       </c>
       <c r="HH2" t="n">
-        <v>0.08774468222100509</v>
+        <v>0.0199046717410412</v>
       </c>
       <c r="HI2" t="n">
-        <v>0.03241370065051732</v>
+        <v>0.03561360694610131</v>
       </c>
       <c r="HJ2" t="n">
-        <v>0.01910305154740542</v>
+        <v>0.03842285068678082</v>
       </c>
       <c r="HK2" t="n">
-        <v>0.02146564891265604</v>
+        <v>0.05357785542540918</v>
       </c>
       <c r="HL2" t="n">
-        <v>0.03551310324748682</v>
+        <v>0.08912738923358349</v>
       </c>
       <c r="HM2" t="n">
-        <v>0.04838935142297955</v>
+        <v>0.07398989919627118</v>
       </c>
       <c r="HN2" t="n">
-        <v>0.07370438459545993</v>
+        <v>0.04410407505348667</v>
       </c>
       <c r="HO2" t="n">
-        <v>0.07133215068844105</v>
+        <v>0.04328887965722945</v>
       </c>
       <c r="HP2" t="n">
-        <v>0.04902060711016702</v>
+        <v>0.03926336180613971</v>
       </c>
       <c r="HQ2" t="n">
-        <v>0.03242441589156513</v>
+        <v>0.07469371358122044</v>
       </c>
       <c r="HR2" t="n">
-        <v>0.03479235804934069</v>
+        <v>0.04131731936847877</v>
       </c>
       <c r="HS2" t="n">
-        <v>0.04999282751258483</v>
+        <v>0.05921380521742607</v>
       </c>
       <c r="HT2" t="n">
-        <v>0.02726235821415722</v>
+        <v>0.03337883655710338</v>
       </c>
       <c r="HU2" t="n">
-        <v>0.04709790415452526</v>
+        <v>0.06225572980482379</v>
       </c>
       <c r="HV2" t="n">
-        <v>0.03573352078187983</v>
+        <v>0.02643766176321629</v>
       </c>
       <c r="HW2" t="n">
-        <v>0.05245949690611423</v>
+        <v>0.05316399928623394</v>
       </c>
       <c r="HX2" t="n">
-        <v>0.02332952810742407</v>
+        <v>0.04281494936174746</v>
       </c>
       <c r="HY2" t="n">
-        <v>0.1808015320660279</v>
+        <v>0.02300379897164192</v>
       </c>
       <c r="HZ2" t="n">
-        <v>0.03314865454974513</v>
+        <v>0.02383773963418142</v>
       </c>
       <c r="IA2" t="n">
-        <v>0.02546903698273702</v>
+        <v>0.04258015234619988</v>
       </c>
       <c r="IB2" t="n">
-        <v>0.04209529388086802</v>
+        <v>0.03896526036581133</v>
       </c>
       <c r="IC2" t="n">
-        <v>0.02314283891313105</v>
+        <v>0.0431193033655678</v>
       </c>
       <c r="ID2" t="n">
-        <v>0.03439076291041252</v>
+        <v>0.03840877366612866</v>
       </c>
       <c r="IE2" t="n">
-        <v>0.03957826372851094</v>
+        <v>0.07491248504452862</v>
       </c>
       <c r="IF2" t="n">
-        <v>0.03369977954472061</v>
+        <v>0.01893415129204472</v>
       </c>
       <c r="IG2" t="n">
-        <v>0.04441893488054769</v>
+        <v>0.1106702718714082</v>
       </c>
       <c r="IH2" t="n">
-        <v>0.0174061644868275</v>
+        <v>0.03103280109603985</v>
       </c>
       <c r="II2" t="n">
-        <v>0.09367899611183607</v>
+        <v>0.01108319913770662</v>
       </c>
       <c r="IJ2" t="n">
-        <v>0.03194838309092859</v>
+        <v>0.02456512316979709</v>
       </c>
       <c r="IK2" t="n">
-        <v>0.01324914169464478</v>
+        <v>0.02109631894950566</v>
       </c>
       <c r="IL2" t="n">
-        <v>0.02917694451246301</v>
+        <v>0.04831435154262356</v>
       </c>
       <c r="IM2" t="n">
-        <v>0.04840480604127519</v>
+        <v>0.05177222293502659</v>
       </c>
       <c r="IN2" t="n">
-        <v>0.04144666752805824</v>
+        <v>0.03198324697258149</v>
       </c>
       <c r="IO2" t="n">
-        <v>0.03960212211365988</v>
+        <v>0.0470993354856867</v>
       </c>
       <c r="IP2" t="n">
-        <v>0.03081681361958447</v>
+        <v>0.05553785475199424</v>
       </c>
       <c r="IQ2" t="n">
-        <v>0.05252929179958721</v>
+        <v>0.0290139859730147</v>
       </c>
       <c r="IR2" t="n">
-        <v>0.07945419911174492</v>
+        <v>0.03770618705101107</v>
       </c>
       <c r="IS2" t="n">
-        <v>0.03348759492689381</v>
+        <v>0.08132309147432096</v>
       </c>
       <c r="IT2" t="n">
-        <v>0.04715049639365185</v>
+        <v>0.03498929534586136</v>
       </c>
       <c r="IU2" t="n">
-        <v>0.07637009518125117</v>
+        <v>0.07088701169710643</v>
       </c>
       <c r="IV2" t="n">
-        <v>0.03081947457283267</v>
+        <v>0.05104746703558175</v>
       </c>
       <c r="IW2" t="n">
-        <v>0.04549220870649565</v>
+        <v>0.03511526790125765</v>
       </c>
       <c r="IX2" t="n">
-        <v>0.05335606396074408</v>
+        <v>0.08137023562483683</v>
       </c>
       <c r="IY2" t="n">
-        <v>0.03013221379126997</v>
+        <v>0.02360704686286185</v>
       </c>
       <c r="IZ2" t="n">
-        <v>0.1274001122791057</v>
+        <v>0.03912106616701236</v>
       </c>
       <c r="JA2" t="n">
-        <v>0.02655878646570822</v>
+        <v>0.1515059249442198</v>
       </c>
       <c r="JB2" t="n">
-        <v>0.03858518426904074</v>
+        <v>0.1051821032258693</v>
       </c>
       <c r="JC2" t="n">
-        <v>0.1183221449463796</v>
+        <v>0.08023855533194778</v>
       </c>
       <c r="JD2" t="n">
-        <v>0.08045852889590244</v>
+        <v>0.04541086337083751</v>
       </c>
       <c r="JE2" t="n">
-        <v>0.1532859687290536</v>
+        <v>0.0385954950094509</v>
       </c>
       <c r="JF2" t="n">
-        <v>0.03081567691046501</v>
+        <v>0.0411327549826374</v>
       </c>
       <c r="JG2" t="n">
-        <v>0.03714044160333259</v>
+        <v>0.06794852623070535</v>
       </c>
       <c r="JH2" t="n">
-        <v>0.02426349320570736</v>
+        <v>0.04709458200786733</v>
       </c>
       <c r="JI2" t="n">
-        <v>0.08790041909369709</v>
+        <v>0.03420754492882029</v>
       </c>
       <c r="JJ2" t="n">
-        <v>0.03956289895346198</v>
+        <v>0.02853352515885156</v>
       </c>
       <c r="JK2" t="n">
-        <v>0.1696195278863661</v>
+        <v>0.03596424131603406</v>
       </c>
       <c r="JL2" t="n">
-        <v>0.07860971105632743</v>
+        <v>0.02893206645133513</v>
       </c>
       <c r="JM2" t="n">
-        <v>0.09193814774892395</v>
+        <v>0.05266877801113964</v>
       </c>
       <c r="JN2" t="n">
-        <v>0.03041976350847539</v>
+        <v>0.08704179382491832</v>
       </c>
       <c r="JO2" t="n">
-        <v>0.05326537834086829</v>
+        <v>0.02720537720537768</v>
       </c>
       <c r="JP2" t="n">
-        <v>0.1665995371786275</v>
+        <v>0.04370069773447267</v>
       </c>
       <c r="JQ2" t="n">
-        <v>0.02266608841333955</v>
+        <v>0.04722243976716239</v>
       </c>
       <c r="JR2" t="n">
-        <v>0.03893262674342887</v>
+        <v>0.05154679682004797</v>
       </c>
       <c r="JS2" t="n">
-        <v>0.04105620875253498</v>
+        <v>0.02651564647826532</v>
       </c>
       <c r="JT2" t="n">
-        <v>0.0339055695796682</v>
+        <v>0.03689339844700416</v>
       </c>
       <c r="JU2" t="n">
-        <v>0.02629237947972616</v>
+        <v>0.04908336873288714</v>
       </c>
       <c r="JV2" t="n">
-        <v>0.03904780131732603</v>
+        <v>0.02125971202616728</v>
       </c>
       <c r="JW2" t="n">
-        <v>0.02378900903296266</v>
+        <v>0.02633604827781508</v>
       </c>
       <c r="JX2" t="n">
-        <v>0.01550086384878979</v>
+        <v>0.04859684671564089</v>
       </c>
       <c r="JY2" t="n">
-        <v>0.02693952335450854</v>
+        <v>0.03410461232648313</v>
       </c>
       <c r="JZ2" t="n">
-        <v>0.04272951263262531</v>
+        <v>0.04795003102847066</v>
       </c>
       <c r="KA2" t="n">
-        <v>0.02614635108680729</v>
+        <v>0.02288734039085856</v>
       </c>
       <c r="KB2" t="n">
-        <v>0.07791401269746541</v>
+        <v>0.03603020905945317</v>
       </c>
       <c r="KC2" t="n">
-        <v>0.02596546645794583</v>
+        <v>0.103742718132854</v>
       </c>
       <c r="KD2" t="n">
-        <v>0.0263465138752658</v>
+        <v>0.05334949256516095</v>
       </c>
       <c r="KE2" t="n">
-        <v>0.07917289666719032</v>
+        <v>0.08033864804604142</v>
       </c>
       <c r="KF2" t="n">
-        <v>0.1455102488156829</v>
+        <v>0.02414694517470082</v>
       </c>
       <c r="KG2" t="n">
-        <v>0.07689758903185791</v>
+        <v>0.03025328957850774</v>
       </c>
       <c r="KH2" t="n">
-        <v>0.02663320870135111</v>
+        <v>0.09317145349610501</v>
       </c>
       <c r="KI2" t="n">
-        <v>0.01667327892298849</v>
+        <v>0.1123742067945531</v>
       </c>
       <c r="KJ2" t="n">
-        <v>0.08012493359304168</v>
+        <v>0.03248239817650357</v>
       </c>
       <c r="KK2" t="n">
-        <v>0.1077426427231309</v>
+        <v>0.1095750893578283</v>
       </c>
       <c r="KL2" t="n">
-        <v>0.03397594475432073</v>
+        <v>0.05794664153554666</v>
       </c>
       <c r="KM2" t="n">
-        <v>0.07279526449549364</v>
+        <v>0.03944839356339584</v>
       </c>
       <c r="KN2" t="n">
-        <v>0.1350848517605365</v>
+        <v>0.04310058970971448</v>
       </c>
       <c r="KO2" t="n">
-        <v>0.03792930201435641</v>
+        <v>0.02475269267668884</v>
       </c>
       <c r="KP2" t="n">
-        <v>0.04431536096540802</v>
+        <v>0.04331987490282509</v>
       </c>
       <c r="KQ2" t="n">
-        <v>0.03113528450434381</v>
+        <v>0.05191400032835749</v>
       </c>
       <c r="KR2" t="n">
-        <v>0.04218265775768351</v>
+        <v>0.02418720442299872</v>
       </c>
       <c r="KS2" t="n">
-        <v>0.04166229747695302</v>
+        <v>0.02268052336281907</v>
       </c>
       <c r="KT2" t="n">
-        <v>0.03674428204951194</v>
+        <v>0.02596257334975007</v>
       </c>
       <c r="KU2" t="n">
-        <v>0.02265659196126922</v>
+        <v>0.0295079964662814</v>
       </c>
       <c r="KV2" t="n">
-        <v>0.02514679528247432</v>
+        <v>0.05077125151633195</v>
       </c>
       <c r="KW2" t="n">
-        <v>0.02759710500615562</v>
+        <v>0.08812496234377262</v>
       </c>
       <c r="KX2" t="n">
-        <v>0.05061298323759104</v>
+        <v>0.01801962957375009</v>
       </c>
       <c r="KY2" t="n">
-        <v>0.1023836006782795</v>
+        <v>0.08321588958105834</v>
       </c>
       <c r="KZ2" t="n">
-        <v>0.02090177860664098</v>
+        <v>0.05051332602205381</v>
       </c>
       <c r="LA2" t="n">
-        <v>0.06034517531796633</v>
+        <v>0.01842235846217914</v>
       </c>
       <c r="LB2" t="n">
-        <v>0.03715493121148754</v>
+        <v>0.1854477860483102</v>
       </c>
       <c r="LC2" t="n">
-        <v>0.0182416921277661</v>
+        <v>0.03359256481844643</v>
       </c>
       <c r="LD2" t="n">
-        <v>0.1400186751097476</v>
+        <v>0.03512654049630833</v>
       </c>
       <c r="LE2" t="n">
-        <v>0.05801629771286287</v>
+        <v>0.02274209104048944</v>
       </c>
       <c r="LF2" t="n">
-        <v>0.0339737660946367</v>
+        <v>0.04336372203853238</v>
       </c>
       <c r="LG2" t="n">
-        <v>0.03027611340750461</v>
+        <v>0.04319967474004811</v>
       </c>
       <c r="LH2" t="n">
-        <v>0.06486745826604649</v>
+        <v>0.1909309713336245</v>
       </c>
       <c r="LI2" t="n">
-        <v>0.1685457298330798</v>
+        <v>0.05069905664009731</v>
       </c>
       <c r="LJ2" t="n">
-        <v>0.05496589344208336</v>
+        <v>0.1018400092706195</v>
       </c>
       <c r="LK2" t="n">
-        <v>0.0846615258888789</v>
+        <v>0.05790609574885715</v>
       </c>
       <c r="LL2" t="n">
-        <v>0.056100555645173</v>
+        <v>0.03380040446113798</v>
       </c>
       <c r="LM2" t="n">
-        <v>0.03190420288429758</v>
+        <v>0.03138803052076181</v>
       </c>
       <c r="LN2" t="n">
-        <v>0.03274086576523018</v>
+        <v>0.08513508283786797</v>
       </c>
       <c r="LO2" t="n">
-        <v>0.06836791768454631</v>
+        <v>0.07152190720549605</v>
       </c>
       <c r="LP2" t="n">
-        <v>0.13494759734827</v>
+        <v>0.1981921317976116</v>
       </c>
       <c r="LQ2" t="n">
-        <v>0.1570978687238508</v>
+        <v>0.05068768281984336</v>
       </c>
       <c r="LR2" t="n">
-        <v>0.07327319821388947</v>
+        <v>0.07787361228451287</v>
       </c>
       <c r="LS2" t="n">
-        <v>0.09564792716956809</v>
+        <v>0.05405954338972716</v>
       </c>
       <c r="LT2" t="n">
-        <v>0.03711745039731236</v>
+        <v>0.03183722325114538</v>
       </c>
       <c r="LU2" t="n">
-        <v>0.04151934439492221</v>
+        <v>0.05826486444621393</v>
       </c>
       <c r="LV2" t="n">
-        <v>0.05733984600668551</v>
+        <v>0.1214139061275</v>
       </c>
       <c r="LW2" t="n">
-        <v>0.1632907719014507</v>
+        <v>0.04556432138707373</v>
       </c>
       <c r="LX2" t="n">
-        <v>0.04633119550929468</v>
+        <v>0.02163638504421271</v>
       </c>
       <c r="LY2" t="n">
-        <v>0.02511894983503817</v>
+        <v>0.05588945013971114</v>
       </c>
       <c r="LZ2" t="n">
-        <v>0.04276560792646473</v>
+        <v>0.02580431015779653</v>
       </c>
       <c r="MA2" t="n">
-        <v>0.01614515493547813</v>
+        <v>0.1043044635731897</v>
       </c>
       <c r="MB2" t="n">
-        <v>0.04802201873517565</v>
+        <v>0.0371047638246443</v>
       </c>
       <c r="MC2" t="n">
-        <v>0.03066950465922908</v>
+        <v>0.06743043493366012</v>
       </c>
       <c r="MD2" t="n">
-        <v>0.03793151136054002</v>
+        <v>0.05822337667409955</v>
       </c>
       <c r="ME2" t="n">
-        <v>0.067367115602931</v>
+        <v>0.02544173551819579</v>
       </c>
       <c r="MF2" t="n">
-        <v>0.01818739909006662</v>
+        <v>0.1530136514004709</v>
       </c>
       <c r="MG2" t="n">
-        <v>0.1427225739919245</v>
+        <v>0.04417809875144121</v>
       </c>
       <c r="MH2" t="n">
-        <v>0.03698884062483441</v>
+        <v>0.07764545198338854</v>
       </c>
       <c r="MI2" t="n">
-        <v>0.07471555545036769</v>
+        <v>0.04138965341622704</v>
       </c>
       <c r="MJ2" t="n">
-        <v>0.03636320756355468</v>
+        <v>0.0499168171167234</v>
       </c>
       <c r="MK2" t="n">
-        <v>0.04492539712276921</v>
+        <v>0.05584991568767679</v>
       </c>
       <c r="ML2" t="n">
-        <v>0.04146683013959662</v>
+        <v>0.05492105657307169</v>
       </c>
       <c r="MM2" t="n">
-        <v>0.03382738914797882</v>
+        <v>0.02187528672635641</v>
       </c>
       <c r="MN2" t="n">
-        <v>0.02286754677137192</v>
+        <v>0.03179172822186488</v>
       </c>
       <c r="MO2" t="n">
-        <v>0.04137182967030768</v>
+        <v>0.03168726924989125</v>
       </c>
       <c r="MP2" t="n">
-        <v>0.02324361958848502</v>
+        <v>0.03764372348913374</v>
       </c>
       <c r="MQ2" t="n">
-        <v>0.02945323121646787</v>
+        <v>0.06404126676881458</v>
       </c>
       <c r="MR2" t="n">
-        <v>0.06390490249977877</v>
+        <v>0.03668674287032408</v>
       </c>
       <c r="MS2" t="n">
-        <v>0.02726199577881932</v>
+        <v>0.02347433405660255</v>
       </c>
       <c r="MT2" t="n">
-        <v>0.03166886064192269</v>
+        <v>0.03000990837998305</v>
       </c>
       <c r="MU2" t="n">
-        <v>0.03919977470236571</v>
+        <v>0.1063886557571182</v>
       </c>
       <c r="MV2" t="n">
-        <v>0.09482129733853911</v>
+        <v>0.1154682956259711</v>
       </c>
       <c r="MW2" t="n">
-        <v>0.1035328146449076</v>
+        <v>0.07748826445109316</v>
       </c>
       <c r="MX2" t="n">
-        <v>0.06369124479881949</v>
+        <v>0.04049119940918501</v>
       </c>
       <c r="MY2" t="n">
-        <v>0.04400792795919424</v>
+        <v>0.036951828288336</v>
       </c>
       <c r="MZ2" t="n">
-        <v>0.02747543670505736</v>
+        <v>0.02625727390000183</v>
       </c>
       <c r="NA2" t="n">
-        <v>0.02854196538094991</v>
+        <v>0.03665690287180277</v>
       </c>
       <c r="NB2" t="n">
-        <v>0.0903409634614421</v>
+        <v>0.0373763804374567</v>
       </c>
       <c r="NC2" t="n">
-        <v>0.03770309292630702</v>
+        <v>0.03946232504194633</v>
       </c>
       <c r="ND2" t="n">
-        <v>0.03229690590212252</v>
+        <v>0.01767579029562025</v>
       </c>
       <c r="NE2" t="n">
-        <v>0.01667718985902917</v>
+        <v>0.08533321200110208</v>
       </c>
       <c r="NF2" t="n">
-        <v>0.06473734728561427</v>
+        <v>0.0697938100326596</v>
       </c>
       <c r="NG2" t="n">
-        <v>0.07209214894791974</v>
+        <v>0.02982558155937438</v>
       </c>
       <c r="NH2" t="n">
-        <v>0.02695086606585908</v>
+        <v>0.0307011100138876</v>
       </c>
       <c r="NI2" t="n">
-        <v>0.0274699776197992</v>
+        <v>0.03742871774562495</v>
       </c>
       <c r="NJ2" t="n">
-        <v>0.03548848759263105</v>
+        <v>0.03446569987003577</v>
       </c>
       <c r="NK2" t="n">
-        <v>0.05259894733711459</v>
+        <v>0.03172024776430951</v>
       </c>
       <c r="NL2" t="n">
-        <v>0.03059122464838211</v>
+        <v>0.0510641865275864</v>
       </c>
       <c r="NM2" t="n">
-        <v>0.03984958925623133</v>
+        <v>0.02244206972631366</v>
       </c>
       <c r="NN2" t="n">
-        <v>0.02164384995826177</v>
+        <v>0.05825312888762735</v>
       </c>
       <c r="NO2" t="n">
-        <v>0.04237403216177677</v>
+        <v>0.02315885671255181</v>
       </c>
       <c r="NP2" t="n">
-        <v>0.02149001162474393</v>
+        <v>0.04081585987576831</v>
       </c>
       <c r="NQ2" t="n">
-        <v>0.03221517069366323</v>
+        <v>0.06967926077831102</v>
       </c>
       <c r="NR2" t="n">
-        <v>0.06578794738912382</v>
+        <v>0.06078349152492098</v>
       </c>
       <c r="NS2" t="n">
-        <v>0.08666718540729183</v>
+        <v>0.1051324251297927</v>
       </c>
       <c r="NT2" t="n">
-        <v>0.06561224403937636</v>
+        <v>0.04860441759560382</v>
       </c>
       <c r="NU2" t="n">
-        <v>0.0765015669264406</v>
+        <v>0.05091616789923212</v>
       </c>
       <c r="NV2" t="n">
-        <v>0.03797973855930645</v>
+        <v>0.08196806742555469</v>
       </c>
       <c r="NW2" t="n">
-        <v>0.05004768180600545</v>
+        <v>0.02151697681578488</v>
       </c>
       <c r="NX2" t="n">
-        <v>0.02013012228076919</v>
+        <v>0.05508698005566313</v>
       </c>
       <c r="NY2" t="n">
-        <v>0.05058583294593475</v>
+        <v>0.07681792842722748</v>
       </c>
       <c r="NZ2" t="n">
-        <v>0.0460193791643334</v>
+        <v>0.03182500960096734</v>
       </c>
       <c r="OA2" t="n">
-        <v>0.03821953373848488</v>
+        <v>0.0137299184133709</v>
       </c>
       <c r="OB2" t="n">
-        <v>0.02739667828287797</v>
+        <v>0.04132339819035701</v>
       </c>
       <c r="OC2" t="n">
-        <v>0.03003256502926709</v>
+        <v>0.01415985184574433</v>
       </c>
       <c r="OD2" t="n">
-        <v>0.05996277110057004</v>
+        <v>0.06817275308500208</v>
       </c>
       <c r="OE2" t="n">
-        <v>0.01685783571070943</v>
+        <v>0.030148104957912</v>
       </c>
       <c r="OF2" t="n">
-        <v>0.04873127391132138</v>
+        <v>0.03647323292380243</v>
       </c>
       <c r="OG2" t="n">
-        <v>0.04947024317139147</v>
+        <v>0.09740219291035905</v>
       </c>
       <c r="OH2" t="n">
-        <v>0.03381380012052553</v>
+        <v>0.02352445790596814</v>
       </c>
       <c r="OI2" t="n">
-        <v>0.131132782136774</v>
+        <v>0.03542186424916936</v>
       </c>
       <c r="OJ2" t="n">
-        <v>0.02288094247085084</v>
+        <v>0.03132527201798347</v>
       </c>
       <c r="OK2" t="n">
-        <v>0.04536072665752049</v>
+        <v>0.05129319707687968</v>
       </c>
       <c r="OL2" t="n">
-        <v>0.02911774964865417</v>
+        <v>0.02167853054569404</v>
       </c>
       <c r="OM2" t="n">
-        <v>0.05709443554756054</v>
+        <v>0.02478384354133035</v>
       </c>
       <c r="ON2" t="n">
-        <v>0.04526821531510444</v>
+        <v>0.08231859182325299</v>
       </c>
       <c r="OO2" t="n">
-        <v>0.01821434166266805</v>
+        <v>0.06290959394697246</v>
       </c>
       <c r="OP2" t="n">
-        <v>0.1217613728991792</v>
+        <v>0.01985887911520835</v>
       </c>
       <c r="OQ2" t="n">
-        <v>0.06237147362285482</v>
+        <v>0.02804985464740391</v>
       </c>
       <c r="OR2" t="n">
-        <v>0.02444050018886467</v>
+        <v>0.0392897003885989</v>
       </c>
       <c r="OS2" t="n">
-        <v>0.02599250900684178</v>
+        <v>0.05462521852182178</v>
       </c>
       <c r="OT2" t="n">
-        <v>0.03166492564442116</v>
+        <v>0.06574208069469509</v>
       </c>
       <c r="OU2" t="n">
-        <v>0.06924664524630568</v>
+        <v>0.07286445279729954</v>
       </c>
       <c r="OV2" t="n">
-        <v>0.0665794801395808</v>
+        <v>0.07724551715481362</v>
       </c>
       <c r="OW2" t="n">
-        <v>0.1296216088391793</v>
+        <v>0.0864695369053349</v>
       </c>
       <c r="OX2" t="n">
-        <v>0.0509905459842878</v>
+        <v>0.0422974523978811</v>
       </c>
       <c r="OY2" t="n">
-        <v>0.07074782907703202</v>
+        <v>0.02024464239667017</v>
       </c>
       <c r="OZ2" t="n">
-        <v>0.03715350930207402</v>
+        <v>0.03571397260793533</v>
       </c>
       <c r="PA2" t="n">
-        <v>0.02215335461271752</v>
+        <v>0.0583588702999839</v>
       </c>
       <c r="PB2" t="n">
-        <v>0.02924028015575537</v>
+        <v>0.02343370182213817</v>
       </c>
       <c r="PC2" t="n">
-        <v>0.03125072525403404</v>
+        <v>0.02799599998268595</v>
       </c>
       <c r="PD2" t="n">
-        <v>0.03342562491323414</v>
+        <v>0.02570587905242543</v>
       </c>
       <c r="PE2" t="n">
-        <v>0.02577151917932461</v>
+        <v>0.04012098703100213</v>
       </c>
       <c r="PF2" t="n">
-        <v>0.03190117868899948</v>
+        <v>0.03526505803162311</v>
       </c>
       <c r="PG2" t="n">
-        <v>0.05850316006315512</v>
+        <v>0.05793241784285681</v>
       </c>
       <c r="PH2" t="n">
-        <v>0.04711867636167409</v>
+        <v>0.05951301395611792</v>
       </c>
       <c r="PI2" t="n">
-        <v>0.08266945887260807</v>
+        <v>0.04072215646627445</v>
       </c>
       <c r="PJ2" t="n">
-        <v>0.03217544936884755</v>
+        <v>0.05625949521684558</v>
       </c>
       <c r="PK2" t="n">
-        <v>0.09961415126224196</v>
+        <v>0.02673464476700181</v>
       </c>
       <c r="PL2" t="n">
-        <v>0.03664995026354879</v>
+        <v>0.04097835570780019</v>
       </c>
       <c r="PM2" t="n">
-        <v>0.06135610446911165</v>
+        <v>0.05093741518161397</v>
       </c>
       <c r="PN2" t="n">
-        <v>0.05730323158602022</v>
+        <v>0.05806208175191067</v>
       </c>
       <c r="PO2" t="n">
-        <v>0.113615343702121</v>
+        <v>0.09344611095490656</v>
       </c>
       <c r="PP2" t="n">
-        <v>0.08499913787777996</v>
+        <v>0.04958267281236146</v>
       </c>
       <c r="PQ2" t="n">
-        <v>0.06183425019461655</v>
+        <v>0.05607393474077029</v>
       </c>
       <c r="PR2" t="n">
-        <v>0.06087847450373457</v>
+        <v>0.06645159673822387</v>
       </c>
       <c r="PS2" t="n">
-        <v>0.06089576404622763</v>
+        <v>0.0395332842327701</v>
       </c>
       <c r="PT2" t="n">
-        <v>0.1084331361947939</v>
+        <v>0.07151907157764745</v>
       </c>
       <c r="PU2" t="n">
-        <v>0.02038067018433851</v>
+        <v>0.02356665815406468</v>
       </c>
       <c r="PV2" t="n">
-        <v>0.05198016549367249</v>
+        <v>0.07479812146462303</v>
       </c>
       <c r="PW2" t="n">
-        <v>0.07475554910493162</v>
+        <v>0.08643339496042519</v>
       </c>
       <c r="PX2" t="n">
-        <v>0.05832127854409114</v>
+        <v>0.05037052940956612</v>
       </c>
       <c r="PY2" t="n">
-        <v>0.0555396479381461</v>
+        <v>0.08930991946962429</v>
       </c>
       <c r="PZ2" t="n">
-        <v>0.03443568860663603</v>
+        <v>0.02814951833029038</v>
       </c>
       <c r="QA2" t="n">
-        <v>0.08368955904812221</v>
+        <v>0.07222894478592352</v>
       </c>
       <c r="QB2" t="n">
-        <v>0.0472620228694912</v>
+        <v>0.03452589595103639</v>
       </c>
       <c r="QC2" t="n">
-        <v>0.02607404666636052</v>
+        <v>0.02155441275836361</v>
       </c>
       <c r="QD2" t="n">
-        <v>0.08087898884842824</v>
+        <v>0.07172553217248381</v>
       </c>
       <c r="QE2" t="n">
-        <v>0.03114407587076408</v>
+        <v>0.03520207344783673</v>
       </c>
       <c r="QF2" t="n">
-        <v>0.1064805323060425</v>
+        <v>0.07777746090851828</v>
       </c>
       <c r="QG2" t="n">
-        <v>0.04787694639868335</v>
+        <v>0.03406430499926506</v>
       </c>
       <c r="QH2" t="n">
-        <v>0.03038625834109826</v>
+        <v>0.04579220544946581</v>
       </c>
       <c r="QI2" t="n">
-        <v>0.03397147946452183</v>
+        <v>0.03311086389139593</v>
       </c>
       <c r="QJ2" t="n">
-        <v>0.02503031875635179</v>
+        <v>0.04603541001266202</v>
       </c>
       <c r="QK2" t="n">
-        <v>0.04397586100881628</v>
+        <v>0.0282890235581129</v>
       </c>
       <c r="QL2" t="n">
-        <v>0.04337212799126718</v>
+        <v>0.05632574137122633</v>
       </c>
       <c r="QM2" t="n">
-        <v>0.0354424687031878</v>
+        <v>0.0363536040369502</v>
       </c>
       <c r="QN2" t="n">
-        <v>0.05123452540958269</v>
+        <v>0.01654887980893652</v>
       </c>
       <c r="QO2" t="n">
-        <v>0.05268292804230322</v>
+        <v>0.04735266326582127</v>
       </c>
       <c r="QP2" t="n">
-        <v>0.03624923967480694</v>
+        <v>0.05558471301131187</v>
       </c>
       <c r="QQ2" t="n">
-        <v>0.02154369962623066</v>
+        <v>0.03055986455603506</v>
       </c>
       <c r="QR2" t="n">
-        <v>0.04792420403410244</v>
+        <v>0.01745706183085336</v>
       </c>
       <c r="QS2" t="n">
-        <v>0.03263907794682078</v>
+        <v>0.06249366785891379</v>
       </c>
       <c r="QT2" t="n">
-        <v>0.03742247264103166</v>
+        <v>0.03122428888095279</v>
       </c>
       <c r="QU2" t="n">
-        <v>0.03470742678300996</v>
+        <v>0.04289249118376871</v>
       </c>
       <c r="QV2" t="n">
-        <v>0.02760469605164486</v>
+        <v>0.04155986393627205</v>
       </c>
       <c r="QW2" t="n">
-        <v>0.02376005926245552</v>
+        <v>0.03689803397260204</v>
       </c>
       <c r="QX2" t="n">
-        <v>0.05175609938408655</v>
+        <v>0.02646306842905414</v>
+      </c>
+      <c r="QY2" t="n">
+        <v>0.05032861862803356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>